<commit_message>
feat: add cardNumber and guideNumber fields to spreadsheet generation
refactor: improve error handling for Google Drive API interactions

fix: update Google Drive configuration redirect URI to use environment variable

feat: enhance spreadsheet form with new fields for cardNumber and guideNumber

style: update spreadsheet preview to display new fields and improve layout

chore: create utility functions for Google Drive API error handling

fix: ensure proper error messages are returned for Google Drive operations

feat: implement reauthorization flow for Google Drive configuration
</commit_message>
<xml_diff>
--- a/src/data/model.xlsx
+++ b/src/data/model.xlsx
@@ -1,26 +1,20 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="21328"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <fileVersion appName="xl" lastEdited="3" lowestEdited="5" rupBuild="9302"/>
   <workbookPr/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Alex Leite\Downloads\"/>
-    </mc:Choice>
-  </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A38EA6CA-F12F-4993-9F75-228197B85E55}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="13176" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView windowWidth="27930" windowHeight="12495"/>
   </bookViews>
   <sheets>
     <sheet name="FREQUÊNCIA" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="191029"/>
+  <calcPr calcId="144525"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="51" uniqueCount="21">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="53" uniqueCount="23">
   <si>
     <t>JP CORPO E MENTE LTDA
 CNPJ: 49.317.168/0001-14
@@ -105,6 +99,12 @@
     </r>
   </si>
   <si>
+    <t xml:space="preserve">Nº carterinha </t>
+  </si>
+  <si>
+    <t>Guia Nº</t>
+  </si>
+  <si>
     <r>
       <rPr>
         <b/>
@@ -127,6 +127,12 @@
       </rPr>
       <t>Data</t>
     </r>
+  </si>
+  <si>
+    <t>Início</t>
+  </si>
+  <si>
+    <t>Final</t>
   </si>
   <si>
     <r>
@@ -200,18 +206,18 @@
       <t>Profissional Executante (Carimbar)</t>
     </r>
   </si>
-  <si>
-    <t>Início</t>
-  </si>
-  <si>
-    <t>Final</t>
-  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="13">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <numFmts count="4">
+    <numFmt numFmtId="176" formatCode="_-* #,##0_-;\-* #,##0_-;_-* &quot;-&quot;_-;_-@_-"/>
+    <numFmt numFmtId="177" formatCode="_-* #,##0.00_-;\-* #,##0.00_-;_-* &quot;-&quot;??_-;_-@_-"/>
+    <numFmt numFmtId="178" formatCode="_-&quot;R$&quot;\ * #,##0.00_-;\-&quot;R$&quot;\ * #,##0.00_-;_-&quot;R$&quot;\ * &quot;-&quot;??_-;_-@_-"/>
+    <numFmt numFmtId="179" formatCode="_-&quot;R$&quot;\ * #,##0_-;\-&quot;R$&quot;\ * #,##0_-;_-&quot;R$&quot;\ * &quot;-&quot;_-;_-@_-"/>
+  </numFmts>
+  <fonts count="33">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -227,12 +233,6 @@
       <charset val="134"/>
     </font>
     <font>
-      <sz val="11"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
       <b/>
       <sz val="12"/>
       <color theme="1"/>
@@ -246,6 +246,12 @@
       <charset val="134"/>
     </font>
     <font>
+      <sz val="11"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
       <b/>
       <sz val="9"/>
       <color theme="1"/>
@@ -253,6 +259,11 @@
       <charset val="134"/>
     </font>
     <font>
+      <sz val="9"/>
+      <name val="Tahoma"/>
+      <charset val="134"/>
+    </font>
+    <font>
       <b/>
       <sz val="8"/>
       <color theme="1"/>
@@ -272,12 +283,6 @@
       <charset val="134"/>
     </font>
     <font>
-      <sz val="8"/>
-      <color theme="1"/>
-      <name val="Tahoma"/>
-      <charset val="134"/>
-    </font>
-    <font>
       <sz val="10"/>
       <color rgb="FF000000"/>
       <name val="Times New Roman"/>
@@ -291,13 +296,163 @@
       <charset val="134"/>
     </font>
     <font>
+      <sz val="8"/>
+      <color theme="1"/>
+      <name val="Tahoma"/>
+      <charset val="134"/>
+    </font>
+    <font>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
       <charset val="134"/>
     </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color rgb="FF0000FF"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFF0000"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="15"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF006100"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF9C0006"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color rgb="FF800080"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="0"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FF3F3F3F"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF3F3F76"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFA7D00"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="13"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FFFA7D00"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF9C6500"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FFFFFFFF"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="18"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <i/>
+      <sz val="11"/>
+      <color rgb="FF7F7F7F"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="9">
+  <fills count="41">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -324,6 +479,12 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor rgb="FFF1F1F1"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor rgb="FFB4C5E7"/>
         <bgColor rgb="FFB4C5E7"/>
       </patternFill>
@@ -346,13 +507,264 @@
         <bgColor rgb="FFDAEEF3"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFC6EFCE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFC7CE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFFCC"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFF2F2F2"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFCC99"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFEB9C"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFA5A5A5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="16">
+  <borders count="27">
     <border>
       <left/>
       <right/>
       <top/>
       <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FFB1B1B1"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color theme="2" tint="-0.249977111117893"/>
+      </left>
+      <right style="thin">
+        <color theme="2" tint="-0.249977111117893"/>
+      </right>
+      <top style="thin">
+        <color theme="2" tint="-0.249977111117893"/>
+      </top>
+      <bottom style="thin">
+        <color theme="2" tint="-0.249977111117893"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FFB1B1B1"/>
+      </left>
+      <right/>
+      <top style="thin">
+        <color rgb="FFB1B1B1"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FFB1B1B1"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color rgb="FFB1B1B1"/>
+      </right>
+      <top style="thin">
+        <color rgb="FFB1B1B1"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FFB1B1B1"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color theme="0" tint="-0.349986266670736"/>
+      </left>
+      <right style="thin">
+        <color theme="0" tint="-0.349986266670736"/>
+      </right>
+      <top style="thin">
+        <color theme="0" tint="-0.349986266670736"/>
+      </top>
+      <bottom style="thin">
+        <color theme="0" tint="-0.349986266670736"/>
+      </bottom>
       <diagonal/>
     </border>
     <border>
@@ -421,9 +833,42 @@
       <diagonal/>
     </border>
     <border>
+      <left style="thin">
+        <color theme="2" tint="-0.249977111117893"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color rgb="FFA5A5A5"/>
+      </right>
+      <top style="thin">
+        <color rgb="FFA5A5A5"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FFA5A5A5"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
       <left style="medium">
         <color rgb="FF000000"/>
       </left>
+      <right/>
+      <top style="medium">
+        <color rgb="FF000000"/>
+      </top>
+      <bottom style="medium">
+        <color rgb="FF000000"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
       <right/>
       <top style="medium">
         <color rgb="FF000000"/>
@@ -446,24 +891,9 @@
     </border>
     <border>
       <left/>
-      <right style="thin">
-        <color rgb="FFA5A5A5"/>
-      </right>
-      <top style="thin">
-        <color rgb="FFA5A5A5"/>
-      </top>
+      <right/>
+      <top/>
       <bottom style="thin">
-        <color rgb="FFA5A5A5"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top style="medium">
-        <color rgb="FF000000"/>
-      </top>
-      <bottom style="medium">
         <color rgb="FF000000"/>
       </bottom>
       <diagonal/>
@@ -483,15 +913,6 @@
     </border>
     <border>
       <left/>
-      <right/>
-      <top/>
-      <bottom style="thin">
-        <color rgb="FF000000"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
       <right style="thin">
         <color rgb="FF000000"/>
       </right>
@@ -502,146 +923,407 @@
       <diagonal/>
     </border>
     <border>
-      <left style="thin">
-        <color rgb="FFB1B1B1"/>
-      </left>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color theme="4"/>
+      </top>
+      <bottom style="double">
+        <color theme="4"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
       <right/>
       <top/>
-      <bottom/>
+      <bottom style="medium">
+        <color theme="4"/>
+      </bottom>
       <diagonal/>
     </border>
     <border>
       <left style="thin">
-        <color theme="2" tint="-0.249977111117893"/>
+        <color rgb="FFB2B2B2"/>
       </left>
-      <right/>
-      <top/>
-      <bottom/>
+      <right style="thin">
+        <color rgb="FFB2B2B2"/>
+      </right>
+      <top style="thin">
+        <color rgb="FFB2B2B2"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FFB2B2B2"/>
+      </bottom>
       <diagonal/>
     </border>
     <border>
       <left style="thin">
-        <color theme="2" tint="-0.249977111117893"/>
+        <color rgb="FF3F3F3F"/>
       </left>
       <right style="thin">
-        <color theme="2" tint="-0.249977111117893"/>
+        <color rgb="FF3F3F3F"/>
       </right>
       <top style="thin">
-        <color theme="2" tint="-0.249977111117893"/>
+        <color rgb="FF3F3F3F"/>
       </top>
       <bottom style="thin">
-        <color theme="2" tint="-0.249977111117893"/>
+        <color rgb="FF3F3F3F"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FF7F7F7F"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF7F7F7F"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF7F7F7F"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF7F7F7F"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="double">
+        <color rgb="FFFF8001"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color theme="4" tint="0.499984740745262"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="double">
+        <color rgb="FF3F3F3F"/>
+      </left>
+      <right style="double">
+        <color rgb="FF3F3F3F"/>
+      </right>
+      <top style="double">
+        <color rgb="FF3F3F3F"/>
+      </top>
+      <bottom style="double">
+        <color rgb="FF3F3F3F"/>
       </bottom>
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="49">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="22" fillId="40" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="35" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="38" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="39" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="25" fillId="0" borderId="24" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="34" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="33" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="37" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="19" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="23" fillId="16" borderId="22" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="178" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="13" borderId="21" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="24" fillId="24" borderId="23" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="28" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="27" fillId="16" borderId="23" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="28" fillId="0" borderId="25" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="32" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="20" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="176" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="31" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="179" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="26" fillId="0" borderId="20" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="177" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="30" fillId="36" borderId="26" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
   </cellStyleXfs>
-  <cellXfs count="36">
+  <cellXfs count="38">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="4" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="5" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="5" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="5" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="6" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="1" fontId="8" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" shrinkToFit="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="7" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" shrinkToFit="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" shrinkToFit="1"/>
+    </xf>
     <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="1" fontId="11" fillId="5" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="7" fillId="6" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="1" fontId="11" fillId="6" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" shrinkToFit="1"/>
     </xf>
-    <xf numFmtId="0" fontId="12" fillId="7" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="5" fillId="6" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="13" fillId="8" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="12" fillId="8" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="13" fillId="9" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="12" fillId="8" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="13" fillId="9" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="12" fillId="8" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="13" fillId="9" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="6" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="5" fillId="5" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="4" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="2" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="4" fillId="4" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="6" fillId="5" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="1" fontId="7" fillId="0" borderId="15" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" shrinkToFit="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="6" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" shrinkToFit="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" shrinkToFit="1"/>
-    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1"/>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="49">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle name="60% - Accent6" xfId="1" builtinId="52"/>
+    <cellStyle name="40% - Accent6" xfId="2" builtinId="51"/>
+    <cellStyle name="60% - Accent5" xfId="3" builtinId="48"/>
+    <cellStyle name="Accent6" xfId="4" builtinId="49"/>
+    <cellStyle name="40% - Accent5" xfId="5" builtinId="47"/>
+    <cellStyle name="20% - Accent5" xfId="6" builtinId="46"/>
+    <cellStyle name="60% - Accent4" xfId="7" builtinId="44"/>
+    <cellStyle name="Accent5" xfId="8" builtinId="45"/>
+    <cellStyle name="40% - Accent4" xfId="9" builtinId="43"/>
+    <cellStyle name="Accent4" xfId="10" builtinId="41"/>
+    <cellStyle name="Linked Cell" xfId="11" builtinId="24"/>
+    <cellStyle name="40% - Accent3" xfId="12" builtinId="39"/>
+    <cellStyle name="60% - Accent2" xfId="13" builtinId="36"/>
+    <cellStyle name="Accent3" xfId="14" builtinId="37"/>
+    <cellStyle name="40% - Accent2" xfId="15" builtinId="35"/>
+    <cellStyle name="20% - Accent2" xfId="16" builtinId="34"/>
+    <cellStyle name="Accent2" xfId="17" builtinId="33"/>
+    <cellStyle name="40% - Accent1" xfId="18" builtinId="31"/>
+    <cellStyle name="20% - Accent1" xfId="19" builtinId="30"/>
+    <cellStyle name="Accent1" xfId="20" builtinId="29"/>
+    <cellStyle name="Neutral" xfId="21" builtinId="28"/>
+    <cellStyle name="60% - Accent1" xfId="22" builtinId="32"/>
+    <cellStyle name="Bad" xfId="23" builtinId="27"/>
+    <cellStyle name="20% - Accent4" xfId="24" builtinId="42"/>
+    <cellStyle name="Total" xfId="25" builtinId="25"/>
+    <cellStyle name="Output" xfId="26" builtinId="21"/>
+    <cellStyle name="Currency" xfId="27" builtinId="4"/>
+    <cellStyle name="20% - Accent3" xfId="28" builtinId="38"/>
+    <cellStyle name="Note" xfId="29" builtinId="10"/>
+    <cellStyle name="Input" xfId="30" builtinId="20"/>
+    <cellStyle name="Heading 4" xfId="31" builtinId="19"/>
+    <cellStyle name="Calculation" xfId="32" builtinId="22"/>
+    <cellStyle name="Good" xfId="33" builtinId="26"/>
+    <cellStyle name="Heading 3" xfId="34" builtinId="18"/>
+    <cellStyle name="CExplanatory Text" xfId="35" builtinId="53"/>
+    <cellStyle name="Heading 1" xfId="36" builtinId="16"/>
+    <cellStyle name="Comma [0]" xfId="37" builtinId="6"/>
+    <cellStyle name="20% - Accent6" xfId="38" builtinId="50"/>
+    <cellStyle name="Title" xfId="39" builtinId="15"/>
+    <cellStyle name="Currency [0]" xfId="40" builtinId="7"/>
+    <cellStyle name="Warning Text" xfId="41" builtinId="11"/>
+    <cellStyle name="Followed Hyperlink" xfId="42" builtinId="9"/>
+    <cellStyle name="Heading 2" xfId="43" builtinId="17"/>
+    <cellStyle name="Comma" xfId="44" builtinId="3"/>
+    <cellStyle name="Check Cell" xfId="45" builtinId="23"/>
+    <cellStyle name="60% - Accent3" xfId="46" builtinId="40"/>
+    <cellStyle name="Percent" xfId="47" builtinId="5"/>
+    <cellStyle name="Hyperlink" xfId="48" builtinId="8"/>
   </cellStyles>
-  <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
-    </ext>
-    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
-      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
     </ext>
   </extLst>
 </styleSheet>
 </file>
 
 <file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
-<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:oneCellAnchor>
     <xdr:from>
       <xdr:col>6</xdr:col>
@@ -652,24 +1334,18 @@
     <xdr:ext cx="1743075" cy="504825"/>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="2" name="image1.png">
-          <a:extLst>
-            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000002000000}"/>
-            </a:ext>
-          </a:extLst>
-        </xdr:cNvPr>
+        <xdr:cNvPr id="2" name="image1.png"/>
         <xdr:cNvPicPr preferRelativeResize="0"/>
       </xdr:nvPicPr>
       <xdr:blipFill>
-        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId1" cstate="print"/>
+        <a:blip r:embed="rId1" cstate="print"/>
         <a:stretch>
           <a:fillRect/>
         </a:stretch>
       </xdr:blipFill>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="6429375" y="104775"/>
+          <a:off x="7047230" y="104775"/>
           <a:ext cx="1743075" cy="504825"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
@@ -875,632 +1551,636 @@
     </a:fmtScheme>
   </a:themeElements>
   <a:objectDefaults/>
-  <a:extraClrSchemeLst/>
 </a:theme>
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
+  <sheetPr/>
   <dimension ref="A1:M1010"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A22" workbookViewId="0">
-      <selection activeCell="J6" sqref="J6"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="H11" sqref="H11"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="14.44140625" defaultRowHeight="15" customHeight="1"/>
+  <sheetFormatPr defaultColWidth="14.4416666666667" defaultRowHeight="15" customHeight="1"/>
   <cols>
     <col min="1" max="1" width="16" customWidth="1"/>
-    <col min="2" max="2" width="15.6640625" customWidth="1"/>
-    <col min="3" max="3" width="12.6640625" customWidth="1"/>
-    <col min="4" max="4" width="13.33203125" customWidth="1"/>
-    <col min="5" max="5" width="14.77734375" customWidth="1"/>
-    <col min="6" max="6" width="8.6640625" customWidth="1"/>
-    <col min="7" max="7" width="40.6640625" customWidth="1"/>
-    <col min="8" max="8" width="23.44140625" customWidth="1"/>
-    <col min="9" max="9" width="15.33203125" customWidth="1"/>
-    <col min="10" max="11" width="8.6640625" customWidth="1"/>
+    <col min="2" max="2" width="15.6666666666667" customWidth="1"/>
+    <col min="3" max="3" width="12.6666666666667" customWidth="1"/>
+    <col min="4" max="4" width="13.3333333333333" customWidth="1"/>
+    <col min="5" max="5" width="14.775" customWidth="1"/>
+    <col min="6" max="6" width="8.66666666666667" customWidth="1"/>
+    <col min="7" max="7" width="40.6666666666667" customWidth="1"/>
+    <col min="8" max="8" width="23.4416666666667" customWidth="1"/>
+    <col min="9" max="9" width="15.3333333333333" customWidth="1"/>
+    <col min="10" max="11" width="8.66666666666667" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:13" ht="61.8" customHeight="1">
-      <c r="A1" s="17" t="s">
+    <row r="1" ht="61.8" customHeight="1" spans="1:8">
+      <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="18"/>
-      <c r="C1" s="18"/>
-      <c r="D1" s="18"/>
-      <c r="E1" s="18"/>
-      <c r="F1" s="18"/>
-      <c r="G1" s="18"/>
-      <c r="H1" s="21"/>
-    </row>
-    <row r="2" spans="1:13" ht="21.75" customHeight="1">
-      <c r="A2" s="19" t="s">
+      <c r="B1" s="2"/>
+      <c r="C1" s="2"/>
+      <c r="D1" s="2"/>
+      <c r="E1" s="2"/>
+      <c r="F1" s="2"/>
+      <c r="G1" s="2"/>
+      <c r="H1" s="25"/>
+    </row>
+    <row r="2" ht="21.75" customHeight="1" spans="1:8">
+      <c r="A2" s="3" t="s">
         <v>1</v>
       </c>
-      <c r="B2" s="20"/>
-      <c r="C2" s="20"/>
-      <c r="D2" s="20"/>
-      <c r="E2" s="20"/>
-      <c r="F2" s="20"/>
-      <c r="G2" s="20"/>
-      <c r="H2" s="21"/>
-    </row>
-    <row r="3" spans="1:13" ht="16.5" customHeight="1">
-      <c r="A3" s="26" t="s">
+      <c r="B2" s="4"/>
+      <c r="C2" s="4"/>
+      <c r="D2" s="4"/>
+      <c r="E2" s="4"/>
+      <c r="F2" s="4"/>
+      <c r="G2" s="4"/>
+      <c r="H2" s="25"/>
+    </row>
+    <row r="3" ht="16.5" customHeight="1" spans="1:8">
+      <c r="A3" s="5" t="s">
         <v>2</v>
       </c>
-      <c r="B3" s="26"/>
-      <c r="C3" s="23"/>
-      <c r="D3" s="23"/>
-      <c r="E3" s="23"/>
-      <c r="F3" s="23"/>
-      <c r="G3" s="23"/>
-      <c r="H3" s="22"/>
-    </row>
-    <row r="4" spans="1:13" ht="16.5" customHeight="1">
-      <c r="A4" s="26" t="s">
+      <c r="B3" s="5"/>
+      <c r="C3" s="6"/>
+      <c r="D3" s="6"/>
+      <c r="E3" s="6"/>
+      <c r="F3" s="6"/>
+      <c r="G3" s="6"/>
+      <c r="H3" s="26"/>
+    </row>
+    <row r="4" ht="16.5" customHeight="1" spans="1:8">
+      <c r="A4" s="5" t="s">
         <v>3</v>
       </c>
-      <c r="B4" s="27"/>
-      <c r="C4" s="23"/>
-      <c r="D4" s="23"/>
-      <c r="E4" s="23"/>
-      <c r="F4" s="23"/>
-      <c r="G4" s="23"/>
-      <c r="H4" s="22"/>
-    </row>
-    <row r="5" spans="1:13" ht="16.5" customHeight="1">
-      <c r="A5" s="28" t="s">
+      <c r="B4" s="7"/>
+      <c r="C4" s="6"/>
+      <c r="D4" s="6"/>
+      <c r="E4" s="6"/>
+      <c r="F4" s="6"/>
+      <c r="G4" s="6"/>
+      <c r="H4" s="26"/>
+    </row>
+    <row r="5" ht="16.5" customHeight="1" spans="1:8">
+      <c r="A5" s="8" t="s">
         <v>4</v>
       </c>
-      <c r="B5" s="27"/>
-      <c r="C5" s="24"/>
-      <c r="D5" s="24"/>
-      <c r="E5" s="24"/>
-      <c r="F5" s="24"/>
-      <c r="G5" s="24"/>
-      <c r="H5" s="22"/>
-    </row>
-    <row r="6" spans="1:13" ht="16.5" customHeight="1">
-      <c r="A6" s="26" t="s">
+      <c r="B5" s="7"/>
+      <c r="C5" s="9"/>
+      <c r="D5" s="9"/>
+      <c r="E5" s="9"/>
+      <c r="F5" s="9"/>
+      <c r="G5" s="9"/>
+      <c r="H5" s="26"/>
+    </row>
+    <row r="6" ht="16.5" customHeight="1" spans="1:8">
+      <c r="A6" s="5" t="s">
         <v>5</v>
       </c>
-      <c r="B6" s="27"/>
-      <c r="C6" s="25"/>
-      <c r="D6" s="25"/>
-      <c r="E6" s="25"/>
-      <c r="F6" s="25"/>
-      <c r="G6" s="25"/>
-      <c r="H6" s="22"/>
-    </row>
-    <row r="7" spans="1:13" ht="16.5" customHeight="1">
-      <c r="A7" s="26" t="s">
+      <c r="B6" s="7"/>
+      <c r="C6" s="10"/>
+      <c r="D6" s="10"/>
+      <c r="E6" s="10"/>
+      <c r="F6" s="10"/>
+      <c r="G6" s="10"/>
+      <c r="H6" s="26"/>
+    </row>
+    <row r="7" ht="16.5" customHeight="1" spans="1:8">
+      <c r="A7" s="5" t="s">
         <v>6</v>
       </c>
-      <c r="B7" s="27"/>
-      <c r="C7" s="23"/>
-      <c r="D7" s="23"/>
-      <c r="E7" s="23"/>
-      <c r="F7" s="23"/>
-      <c r="G7" s="23"/>
-      <c r="H7" s="22"/>
-    </row>
-    <row r="8" spans="1:13" ht="16.5" customHeight="1">
-      <c r="A8" s="26" t="s">
+      <c r="B7" s="7"/>
+      <c r="C7" s="6"/>
+      <c r="D7" s="6"/>
+      <c r="E7" s="6"/>
+      <c r="F7" s="6"/>
+      <c r="G7" s="6"/>
+      <c r="H7" s="26"/>
+    </row>
+    <row r="8" ht="16.5" customHeight="1" spans="1:8">
+      <c r="A8" s="5" t="s">
         <v>7</v>
       </c>
-      <c r="B8" s="27"/>
-      <c r="C8" s="23"/>
-      <c r="D8" s="23"/>
-      <c r="E8" s="23"/>
-      <c r="F8" s="23"/>
-      <c r="G8" s="23"/>
-      <c r="H8" s="22"/>
-    </row>
-    <row r="9" spans="1:13" ht="12.75" customHeight="1">
-      <c r="A9" s="29"/>
-      <c r="B9" s="29"/>
-      <c r="C9" s="29"/>
-      <c r="D9" s="29"/>
-      <c r="E9" s="29"/>
-      <c r="F9" s="29"/>
-      <c r="G9" s="29"/>
-    </row>
-    <row r="10" spans="1:13" ht="12.75" customHeight="1">
-      <c r="A10" s="29"/>
-      <c r="B10" s="29"/>
-      <c r="C10" s="29"/>
-      <c r="D10" s="29"/>
-      <c r="E10" s="29"/>
-      <c r="F10" s="29"/>
-      <c r="G10" s="29"/>
-    </row>
-    <row r="11" spans="1:13" ht="19.5" customHeight="1">
-      <c r="A11" s="30" t="s">
+      <c r="B8" s="7"/>
+      <c r="C8" s="6"/>
+      <c r="D8" s="6"/>
+      <c r="E8" s="6"/>
+      <c r="F8" s="6"/>
+      <c r="G8" s="6"/>
+      <c r="H8" s="26"/>
+    </row>
+    <row r="9" ht="12.75" customHeight="1" spans="1:7">
+      <c r="A9" s="11" t="s">
         <v>8</v>
       </c>
-      <c r="B11" s="30" t="s">
+      <c r="B9" s="12"/>
+      <c r="C9" s="6"/>
+      <c r="D9" s="6"/>
+      <c r="E9" s="6"/>
+      <c r="F9" s="6"/>
+      <c r="G9" s="6"/>
+    </row>
+    <row r="10" ht="12.75" customHeight="1" spans="1:7">
+      <c r="A10" s="13" t="s">
         <v>9</v>
       </c>
-      <c r="C11" s="30" t="s">
+      <c r="B10" s="13"/>
+      <c r="C10" s="6"/>
+      <c r="D10" s="6"/>
+      <c r="E10" s="6"/>
+      <c r="F10" s="6"/>
+      <c r="G10" s="6"/>
+    </row>
+    <row r="11" ht="19.5" customHeight="1"/>
+    <row r="12" ht="19.5" customHeight="1" spans="1:7">
+      <c r="A12" s="14" t="s">
+        <v>10</v>
+      </c>
+      <c r="B12" s="14" t="s">
+        <v>11</v>
+      </c>
+      <c r="C12" s="14" t="s">
+        <v>12</v>
+      </c>
+      <c r="D12" s="14" t="s">
+        <v>13</v>
+      </c>
+      <c r="E12" s="14" t="s">
+        <v>14</v>
+      </c>
+      <c r="F12" s="14" t="s">
+        <v>15</v>
+      </c>
+      <c r="G12" s="14" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="13" ht="19.5" customHeight="1" spans="1:13">
+      <c r="A13" s="15">
+        <v>1</v>
+      </c>
+      <c r="B13" s="16"/>
+      <c r="C13" s="16"/>
+      <c r="D13" s="16"/>
+      <c r="E13" s="15"/>
+      <c r="F13" s="27" t="s">
+        <v>17</v>
+      </c>
+      <c r="G13" s="28"/>
+      <c r="J13" s="30" t="s">
+        <v>18</v>
+      </c>
+      <c r="K13" s="31"/>
+      <c r="L13" s="31"/>
+      <c r="M13" s="35"/>
+    </row>
+    <row r="14" ht="19.5" customHeight="1" spans="1:13">
+      <c r="A14" s="15">
+        <v>2</v>
+      </c>
+      <c r="B14" s="16"/>
+      <c r="C14" s="16"/>
+      <c r="D14" s="16"/>
+      <c r="E14" s="15"/>
+      <c r="F14" s="27" t="s">
+        <v>17</v>
+      </c>
+      <c r="G14" s="28"/>
+      <c r="J14" s="32"/>
+      <c r="K14" s="33"/>
+      <c r="L14" s="33"/>
+      <c r="M14" s="36"/>
+    </row>
+    <row r="15" ht="19.5" customHeight="1" spans="1:7">
+      <c r="A15" s="15">
+        <v>3</v>
+      </c>
+      <c r="B15" s="17"/>
+      <c r="C15" s="17"/>
+      <c r="D15" s="17"/>
+      <c r="E15" s="15"/>
+      <c r="F15" s="27" t="s">
+        <v>17</v>
+      </c>
+      <c r="G15" s="28"/>
+    </row>
+    <row r="16" ht="19.5" customHeight="1" spans="1:13">
+      <c r="A16" s="15">
+        <v>4</v>
+      </c>
+      <c r="B16" s="17"/>
+      <c r="C16" s="17"/>
+      <c r="D16" s="17"/>
+      <c r="E16" s="15"/>
+      <c r="F16" s="27" t="s">
+        <v>17</v>
+      </c>
+      <c r="G16" s="28"/>
+      <c r="J16" s="30" t="s">
         <v>19</v>
       </c>
-      <c r="D11" s="30" t="s">
+      <c r="K16" s="31"/>
+      <c r="L16" s="31"/>
+      <c r="M16" s="35"/>
+    </row>
+    <row r="17" ht="19.5" customHeight="1" spans="1:13">
+      <c r="A17" s="15">
+        <v>5</v>
+      </c>
+      <c r="B17" s="17"/>
+      <c r="C17" s="17"/>
+      <c r="D17" s="17"/>
+      <c r="E17" s="15"/>
+      <c r="F17" s="27" t="s">
+        <v>17</v>
+      </c>
+      <c r="G17" s="28"/>
+      <c r="J17" s="32"/>
+      <c r="K17" s="34"/>
+      <c r="L17" s="34"/>
+      <c r="M17" s="37"/>
+    </row>
+    <row r="18" ht="19.5" customHeight="1" spans="1:7">
+      <c r="A18" s="15">
+        <v>6</v>
+      </c>
+      <c r="B18" s="17"/>
+      <c r="C18" s="17"/>
+      <c r="D18" s="17"/>
+      <c r="E18" s="15"/>
+      <c r="F18" s="27" t="s">
+        <v>17</v>
+      </c>
+      <c r="G18" s="28"/>
+    </row>
+    <row r="19" ht="19.5" customHeight="1" spans="1:13">
+      <c r="A19" s="15">
+        <v>7</v>
+      </c>
+      <c r="B19" s="17"/>
+      <c r="C19" s="17"/>
+      <c r="D19" s="17"/>
+      <c r="E19" s="15"/>
+      <c r="F19" s="27" t="s">
+        <v>17</v>
+      </c>
+      <c r="G19" s="28"/>
+      <c r="J19" s="30" t="s">
         <v>20</v>
       </c>
-      <c r="E11" s="30" t="s">
+      <c r="K19" s="31"/>
+      <c r="L19" s="31"/>
+      <c r="M19" s="35"/>
+    </row>
+    <row r="20" ht="19.5" customHeight="1" spans="1:13">
+      <c r="A20" s="15">
+        <v>8</v>
+      </c>
+      <c r="B20" s="17"/>
+      <c r="C20" s="17"/>
+      <c r="D20" s="17"/>
+      <c r="E20" s="15"/>
+      <c r="F20" s="27" t="s">
+        <v>17</v>
+      </c>
+      <c r="G20" s="28"/>
+      <c r="J20" s="32"/>
+      <c r="K20" s="33"/>
+      <c r="L20" s="33"/>
+      <c r="M20" s="36"/>
+    </row>
+    <row r="21" ht="19.5" customHeight="1" spans="1:7">
+      <c r="A21" s="15">
+        <v>9</v>
+      </c>
+      <c r="B21" s="17"/>
+      <c r="C21" s="17"/>
+      <c r="D21" s="17"/>
+      <c r="E21" s="15"/>
+      <c r="F21" s="27" t="s">
+        <v>17</v>
+      </c>
+      <c r="G21" s="28"/>
+    </row>
+    <row r="22" ht="19.5" customHeight="1" spans="1:7">
+      <c r="A22" s="15">
         <v>10</v>
       </c>
-      <c r="F11" s="30" t="s">
+      <c r="B22" s="17"/>
+      <c r="C22" s="17"/>
+      <c r="D22" s="17"/>
+      <c r="E22" s="15"/>
+      <c r="F22" s="27" t="s">
+        <v>17</v>
+      </c>
+      <c r="G22" s="28"/>
+    </row>
+    <row r="23" ht="19.5" customHeight="1" spans="1:7">
+      <c r="A23" s="15">
         <v>11</v>
       </c>
-      <c r="G11" s="30" t="s">
+      <c r="B23" s="17"/>
+      <c r="C23" s="17"/>
+      <c r="D23" s="17"/>
+      <c r="E23" s="15"/>
+      <c r="F23" s="27" t="s">
+        <v>17</v>
+      </c>
+      <c r="G23" s="28"/>
+    </row>
+    <row r="24" ht="19.5" customHeight="1" spans="1:7">
+      <c r="A24" s="15">
         <v>12</v>
       </c>
-    </row>
-    <row r="12" spans="1:13" ht="19.5" customHeight="1" thickBot="1">
-      <c r="A12" s="31">
-        <v>1</v>
-      </c>
-      <c r="B12" s="32"/>
-      <c r="C12" s="32"/>
-      <c r="D12" s="32"/>
-      <c r="E12" s="31"/>
-      <c r="F12" s="33" t="s">
+      <c r="B24" s="17"/>
+      <c r="C24" s="17"/>
+      <c r="D24" s="17"/>
+      <c r="E24" s="15"/>
+      <c r="F24" s="27" t="s">
+        <v>17</v>
+      </c>
+      <c r="G24" s="28"/>
+    </row>
+    <row r="25" ht="19.5" customHeight="1" spans="1:7">
+      <c r="A25" s="15">
         <v>13</v>
       </c>
-      <c r="G12" s="34"/>
-    </row>
-    <row r="13" spans="1:13" ht="19.5" customHeight="1" thickBot="1">
-      <c r="A13" s="31">
-        <v>2</v>
-      </c>
-      <c r="B13" s="32"/>
-      <c r="C13" s="32"/>
-      <c r="D13" s="32"/>
-      <c r="E13" s="31"/>
-      <c r="F13" s="33" t="s">
-        <v>13</v>
-      </c>
-      <c r="G13" s="34"/>
-      <c r="J13" s="3" t="s">
+      <c r="B25" s="17"/>
+      <c r="C25" s="17"/>
+      <c r="D25" s="17"/>
+      <c r="E25" s="15"/>
+      <c r="F25" s="27" t="s">
+        <v>17</v>
+      </c>
+      <c r="G25" s="28"/>
+    </row>
+    <row r="26" ht="19.5" customHeight="1" spans="1:7">
+      <c r="A26" s="15">
         <v>14</v>
       </c>
-      <c r="K13" s="4"/>
-      <c r="L13" s="4"/>
-      <c r="M13" s="5"/>
-    </row>
-    <row r="14" spans="1:13" ht="19.5" customHeight="1">
-      <c r="A14" s="31">
-        <v>3</v>
-      </c>
-      <c r="B14" s="35"/>
-      <c r="C14" s="35"/>
-      <c r="D14" s="35"/>
-      <c r="E14" s="31"/>
-      <c r="F14" s="33" t="s">
-        <v>13</v>
-      </c>
-      <c r="G14" s="34"/>
-      <c r="J14" s="6"/>
-      <c r="K14" s="7"/>
-      <c r="L14" s="7"/>
-      <c r="M14" s="8"/>
-    </row>
-    <row r="15" spans="1:13" ht="19.5" customHeight="1" thickBot="1">
-      <c r="A15" s="31">
-        <v>4</v>
-      </c>
-      <c r="B15" s="35"/>
-      <c r="C15" s="35"/>
-      <c r="D15" s="35"/>
-      <c r="E15" s="31"/>
-      <c r="F15" s="33" t="s">
-        <v>13</v>
-      </c>
-      <c r="G15" s="34"/>
-    </row>
-    <row r="16" spans="1:13" ht="19.5" customHeight="1" thickBot="1">
-      <c r="A16" s="31">
-        <v>5</v>
-      </c>
-      <c r="B16" s="35"/>
-      <c r="C16" s="35"/>
-      <c r="D16" s="35"/>
-      <c r="E16" s="31"/>
-      <c r="F16" s="33" t="s">
-        <v>13</v>
-      </c>
-      <c r="G16" s="34"/>
-      <c r="J16" s="3" t="s">
+      <c r="B26" s="17"/>
+      <c r="C26" s="17"/>
+      <c r="D26" s="17"/>
+      <c r="E26" s="15"/>
+      <c r="F26" s="27" t="s">
+        <v>17</v>
+      </c>
+      <c r="G26" s="28"/>
+    </row>
+    <row r="27" ht="19.5" customHeight="1" spans="1:7">
+      <c r="A27" s="15">
         <v>15</v>
       </c>
-      <c r="K16" s="4"/>
-      <c r="L16" s="4"/>
-      <c r="M16" s="5"/>
-    </row>
-    <row r="17" spans="1:13" ht="19.5" customHeight="1">
-      <c r="A17" s="31">
-        <v>6</v>
-      </c>
-      <c r="B17" s="35"/>
-      <c r="C17" s="35"/>
-      <c r="D17" s="35"/>
-      <c r="E17" s="31"/>
-      <c r="F17" s="33" t="s">
-        <v>13</v>
-      </c>
-      <c r="G17" s="34"/>
-      <c r="J17" s="6"/>
-      <c r="K17" s="9"/>
-      <c r="L17" s="9"/>
-      <c r="M17" s="10"/>
-    </row>
-    <row r="18" spans="1:13" ht="19.5" customHeight="1" thickBot="1">
-      <c r="A18" s="31">
-        <v>7</v>
-      </c>
-      <c r="B18" s="35"/>
-      <c r="C18" s="35"/>
-      <c r="D18" s="35"/>
-      <c r="E18" s="31"/>
-      <c r="F18" s="33" t="s">
-        <v>13</v>
-      </c>
-      <c r="G18" s="34"/>
-    </row>
-    <row r="19" spans="1:13" ht="19.5" customHeight="1" thickBot="1">
-      <c r="A19" s="31">
-        <v>8</v>
-      </c>
-      <c r="B19" s="35"/>
-      <c r="C19" s="35"/>
-      <c r="D19" s="35"/>
-      <c r="E19" s="31"/>
-      <c r="F19" s="33" t="s">
-        <v>13</v>
-      </c>
-      <c r="G19" s="34"/>
-      <c r="J19" s="3" t="s">
+      <c r="B27" s="17"/>
+      <c r="C27" s="17"/>
+      <c r="D27" s="17"/>
+      <c r="E27" s="15"/>
+      <c r="F27" s="27" t="s">
+        <v>17</v>
+      </c>
+      <c r="G27" s="28"/>
+    </row>
+    <row r="28" ht="19.5" customHeight="1" spans="1:7">
+      <c r="A28" s="15">
         <v>16</v>
       </c>
-      <c r="K19" s="4"/>
-      <c r="L19" s="4"/>
-      <c r="M19" s="5"/>
-    </row>
-    <row r="20" spans="1:13" ht="19.5" customHeight="1">
-      <c r="A20" s="31">
-        <v>9</v>
-      </c>
-      <c r="B20" s="35"/>
-      <c r="C20" s="35"/>
-      <c r="D20" s="35"/>
-      <c r="E20" s="31"/>
-      <c r="F20" s="33" t="s">
-        <v>13</v>
-      </c>
-      <c r="G20" s="34"/>
-      <c r="J20" s="6"/>
-      <c r="K20" s="7"/>
-      <c r="L20" s="7"/>
-      <c r="M20" s="8"/>
-    </row>
-    <row r="21" spans="1:13" ht="19.5" customHeight="1">
-      <c r="A21" s="31">
-        <v>10</v>
-      </c>
-      <c r="B21" s="35"/>
-      <c r="C21" s="35"/>
-      <c r="D21" s="35"/>
-      <c r="E21" s="31"/>
-      <c r="F21" s="33" t="s">
-        <v>13</v>
-      </c>
-      <c r="G21" s="34"/>
-    </row>
-    <row r="22" spans="1:13" ht="19.5" customHeight="1">
-      <c r="A22" s="31">
-        <v>11</v>
-      </c>
-      <c r="B22" s="35"/>
-      <c r="C22" s="35"/>
-      <c r="D22" s="35"/>
-      <c r="E22" s="31"/>
-      <c r="F22" s="33" t="s">
-        <v>13</v>
-      </c>
-      <c r="G22" s="34"/>
-    </row>
-    <row r="23" spans="1:13" ht="19.5" customHeight="1">
-      <c r="A23" s="31">
-        <v>12</v>
-      </c>
-      <c r="B23" s="35"/>
-      <c r="C23" s="35"/>
-      <c r="D23" s="35"/>
-      <c r="E23" s="31"/>
-      <c r="F23" s="33" t="s">
-        <v>13</v>
-      </c>
-      <c r="G23" s="34"/>
-    </row>
-    <row r="24" spans="1:13" ht="19.5" customHeight="1">
-      <c r="A24" s="31">
-        <v>13</v>
-      </c>
-      <c r="B24" s="35"/>
-      <c r="C24" s="35"/>
-      <c r="D24" s="35"/>
-      <c r="E24" s="31"/>
-      <c r="F24" s="33" t="s">
-        <v>13</v>
-      </c>
-      <c r="G24" s="34"/>
-    </row>
-    <row r="25" spans="1:13" ht="19.5" customHeight="1">
-      <c r="A25" s="31">
-        <v>14</v>
-      </c>
-      <c r="B25" s="35"/>
-      <c r="C25" s="35"/>
-      <c r="D25" s="35"/>
-      <c r="E25" s="31"/>
-      <c r="F25" s="33" t="s">
-        <v>13</v>
-      </c>
-      <c r="G25" s="34"/>
-    </row>
-    <row r="26" spans="1:13" ht="19.5" customHeight="1">
-      <c r="A26" s="31">
-        <v>15</v>
-      </c>
-      <c r="B26" s="35"/>
-      <c r="C26" s="35"/>
-      <c r="D26" s="35"/>
-      <c r="E26" s="31"/>
-      <c r="F26" s="33" t="s">
-        <v>13</v>
-      </c>
-      <c r="G26" s="34"/>
-    </row>
-    <row r="27" spans="1:13" ht="19.5" customHeight="1">
-      <c r="A27" s="31">
-        <v>16</v>
-      </c>
-      <c r="B27" s="35"/>
-      <c r="C27" s="35"/>
-      <c r="D27" s="35"/>
-      <c r="E27" s="31"/>
-      <c r="F27" s="33" t="s">
-        <v>13</v>
-      </c>
-      <c r="G27" s="34"/>
-    </row>
-    <row r="28" spans="1:13" ht="19.5" customHeight="1">
-      <c r="A28" s="31">
+      <c r="B28" s="17"/>
+      <c r="C28" s="17"/>
+      <c r="D28" s="17"/>
+      <c r="E28" s="15"/>
+      <c r="F28" s="27" t="s">
         <v>17</v>
       </c>
-      <c r="B28" s="35"/>
-      <c r="C28" s="35"/>
-      <c r="D28" s="35"/>
-      <c r="E28" s="31"/>
-      <c r="F28" s="33" t="s">
-        <v>13</v>
-      </c>
-      <c r="G28" s="34"/>
-    </row>
-    <row r="29" spans="1:13" ht="19.5" customHeight="1">
-      <c r="A29" s="31">
+      <c r="G28" s="28"/>
+    </row>
+    <row r="29" ht="19.5" customHeight="1" spans="1:7">
+      <c r="A29" s="15">
+        <v>17</v>
+      </c>
+      <c r="B29" s="17"/>
+      <c r="C29" s="17"/>
+      <c r="D29" s="17"/>
+      <c r="E29" s="15"/>
+      <c r="F29" s="27" t="s">
+        <v>17</v>
+      </c>
+      <c r="G29" s="28"/>
+    </row>
+    <row r="30" ht="19.5" customHeight="1" spans="1:7">
+      <c r="A30" s="15">
         <v>18</v>
       </c>
-      <c r="B29" s="35"/>
-      <c r="C29" s="35"/>
-      <c r="D29" s="35"/>
-      <c r="E29" s="31"/>
-      <c r="F29" s="33" t="s">
-        <v>13</v>
-      </c>
-      <c r="G29" s="34"/>
-    </row>
-    <row r="30" spans="1:13" ht="19.5" customHeight="1">
-      <c r="A30" s="31">
+      <c r="B30" s="17"/>
+      <c r="C30" s="17"/>
+      <c r="D30" s="17"/>
+      <c r="E30" s="15"/>
+      <c r="F30" s="27" t="s">
+        <v>17</v>
+      </c>
+      <c r="G30" s="28"/>
+    </row>
+    <row r="31" ht="19.5" customHeight="1" spans="1:7">
+      <c r="A31" s="15">
         <v>19</v>
       </c>
-      <c r="B30" s="35"/>
-      <c r="C30" s="35"/>
-      <c r="D30" s="35"/>
-      <c r="E30" s="31"/>
-      <c r="F30" s="33" t="s">
-        <v>13</v>
-      </c>
-      <c r="G30" s="34"/>
-    </row>
-    <row r="31" spans="1:13" ht="19.5" customHeight="1">
-      <c r="A31" s="31">
+      <c r="B31" s="17"/>
+      <c r="C31" s="17"/>
+      <c r="D31" s="17"/>
+      <c r="E31" s="15"/>
+      <c r="F31" s="27" t="s">
+        <v>17</v>
+      </c>
+      <c r="G31" s="28"/>
+    </row>
+    <row r="32" ht="19.5" customHeight="1" spans="1:7">
+      <c r="A32" s="15">
         <v>20</v>
       </c>
-      <c r="B31" s="35"/>
-      <c r="C31" s="35"/>
-      <c r="D31" s="35"/>
-      <c r="E31" s="31"/>
-      <c r="F31" s="33" t="s">
-        <v>13</v>
-      </c>
-      <c r="G31" s="34"/>
-    </row>
-    <row r="32" spans="1:13" ht="19.5" customHeight="1">
-      <c r="A32" s="31">
+      <c r="B32" s="17"/>
+      <c r="C32" s="17"/>
+      <c r="D32" s="17"/>
+      <c r="E32" s="15"/>
+      <c r="F32" s="27" t="s">
+        <v>17</v>
+      </c>
+      <c r="G32" s="28"/>
+    </row>
+    <row r="33" ht="19.5" customHeight="1" spans="1:7">
+      <c r="A33" s="15">
         <v>21</v>
       </c>
-      <c r="B32" s="35"/>
-      <c r="C32" s="35"/>
-      <c r="D32" s="35"/>
-      <c r="E32" s="31"/>
-      <c r="F32" s="33" t="s">
-        <v>13</v>
-      </c>
-      <c r="G32" s="34"/>
-    </row>
-    <row r="33" spans="1:7" ht="19.5" customHeight="1">
-      <c r="A33" s="31">
+      <c r="B33" s="17"/>
+      <c r="C33" s="17"/>
+      <c r="D33" s="17"/>
+      <c r="E33" s="15"/>
+      <c r="F33" s="27" t="s">
+        <v>17</v>
+      </c>
+      <c r="G33" s="28"/>
+    </row>
+    <row r="34" ht="19.5" customHeight="1" spans="1:7">
+      <c r="A34" s="15">
         <v>22</v>
       </c>
-      <c r="B33" s="35"/>
-      <c r="C33" s="35"/>
-      <c r="D33" s="35"/>
-      <c r="E33" s="31"/>
-      <c r="F33" s="33" t="s">
-        <v>13</v>
-      </c>
-      <c r="G33" s="34"/>
-    </row>
-    <row r="34" spans="1:7" ht="19.5" customHeight="1">
-      <c r="A34" s="31">
+      <c r="B34" s="17"/>
+      <c r="C34" s="17"/>
+      <c r="D34" s="17"/>
+      <c r="E34" s="15"/>
+      <c r="F34" s="27" t="s">
+        <v>17</v>
+      </c>
+      <c r="G34" s="28"/>
+    </row>
+    <row r="35" ht="19.5" customHeight="1" spans="1:7">
+      <c r="A35" s="15">
         <v>23</v>
       </c>
-      <c r="B34" s="35"/>
-      <c r="C34" s="35"/>
-      <c r="D34" s="35"/>
-      <c r="E34" s="31"/>
-      <c r="F34" s="33" t="s">
-        <v>13</v>
-      </c>
-      <c r="G34" s="34"/>
-    </row>
-    <row r="35" spans="1:7" ht="19.5" customHeight="1">
-      <c r="A35" s="31">
+      <c r="B35" s="17"/>
+      <c r="C35" s="17"/>
+      <c r="D35" s="17"/>
+      <c r="E35" s="15"/>
+      <c r="F35" s="27" t="s">
+        <v>17</v>
+      </c>
+      <c r="G35" s="28"/>
+    </row>
+    <row r="36" ht="19.5" customHeight="1" spans="1:7">
+      <c r="A36" s="15">
         <v>24</v>
       </c>
-      <c r="B35" s="35"/>
-      <c r="C35" s="35"/>
-      <c r="D35" s="35"/>
-      <c r="E35" s="31"/>
-      <c r="F35" s="33" t="s">
-        <v>13</v>
-      </c>
-      <c r="G35" s="34"/>
-    </row>
-    <row r="36" spans="1:7" ht="19.5" customHeight="1">
-      <c r="A36" s="31">
+      <c r="B36" s="17"/>
+      <c r="C36" s="17"/>
+      <c r="D36" s="17"/>
+      <c r="E36" s="15"/>
+      <c r="F36" s="27" t="s">
+        <v>17</v>
+      </c>
+      <c r="G36" s="28"/>
+    </row>
+    <row r="37" ht="19.5" customHeight="1" spans="1:7">
+      <c r="A37" s="15">
         <v>25</v>
       </c>
-      <c r="B36" s="35"/>
-      <c r="C36" s="35"/>
-      <c r="D36" s="35"/>
-      <c r="E36" s="31"/>
-      <c r="F36" s="33" t="s">
-        <v>13</v>
-      </c>
-      <c r="G36" s="34"/>
-    </row>
-    <row r="37" spans="1:7" ht="19.5" customHeight="1">
-      <c r="A37" s="31">
+      <c r="B37" s="17"/>
+      <c r="C37" s="17"/>
+      <c r="D37" s="17"/>
+      <c r="E37" s="15"/>
+      <c r="F37" s="27" t="s">
+        <v>17</v>
+      </c>
+      <c r="G37" s="28"/>
+    </row>
+    <row r="38" ht="19.5" customHeight="1" spans="1:7">
+      <c r="A38" s="15">
         <v>26</v>
       </c>
-      <c r="B37" s="35"/>
-      <c r="C37" s="35"/>
-      <c r="D37" s="35"/>
-      <c r="E37" s="31"/>
-      <c r="F37" s="33" t="s">
-        <v>13</v>
-      </c>
-      <c r="G37" s="34"/>
-    </row>
-    <row r="38" spans="1:7" ht="19.5" customHeight="1">
-      <c r="A38" s="31">
+      <c r="B38" s="17"/>
+      <c r="C38" s="17"/>
+      <c r="D38" s="17"/>
+      <c r="E38" s="15"/>
+      <c r="F38" s="27" t="s">
+        <v>17</v>
+      </c>
+      <c r="G38" s="28"/>
+    </row>
+    <row r="39" ht="19.5" customHeight="1" spans="1:7">
+      <c r="A39" s="15">
         <v>27</v>
       </c>
-      <c r="B38" s="35"/>
-      <c r="C38" s="35"/>
-      <c r="D38" s="35"/>
-      <c r="E38" s="31"/>
-      <c r="F38" s="33" t="s">
-        <v>13</v>
-      </c>
-      <c r="G38" s="34"/>
-    </row>
-    <row r="39" spans="1:7" ht="19.5" customHeight="1">
-      <c r="A39" s="31">
+      <c r="B39" s="17"/>
+      <c r="C39" s="17"/>
+      <c r="D39" s="17"/>
+      <c r="E39" s="15"/>
+      <c r="F39" s="27" t="s">
+        <v>17</v>
+      </c>
+      <c r="G39" s="28"/>
+    </row>
+    <row r="40" ht="19.5" customHeight="1" spans="1:7">
+      <c r="A40" s="15">
         <v>28</v>
       </c>
-      <c r="B39" s="35"/>
-      <c r="C39" s="35"/>
-      <c r="D39" s="35"/>
-      <c r="E39" s="31"/>
-      <c r="F39" s="33" t="s">
-        <v>13</v>
-      </c>
-      <c r="G39" s="34"/>
-    </row>
-    <row r="40" spans="1:7" ht="19.5" customHeight="1">
-      <c r="A40" s="31">
+      <c r="B40" s="17"/>
+      <c r="C40" s="17"/>
+      <c r="D40" s="17"/>
+      <c r="E40" s="15"/>
+      <c r="F40" s="27" t="s">
+        <v>17</v>
+      </c>
+      <c r="G40" s="28"/>
+    </row>
+    <row r="41" ht="19.5" customHeight="1" spans="1:7">
+      <c r="A41" s="15">
         <v>29</v>
       </c>
-      <c r="B40" s="35"/>
-      <c r="C40" s="35"/>
-      <c r="D40" s="35"/>
-      <c r="E40" s="31"/>
-      <c r="F40" s="33" t="s">
-        <v>13</v>
-      </c>
-      <c r="G40" s="34"/>
-    </row>
-    <row r="41" spans="1:7" ht="19.5" customHeight="1">
-      <c r="A41" s="31">
+      <c r="B41" s="17"/>
+      <c r="C41" s="17"/>
+      <c r="D41" s="17"/>
+      <c r="E41" s="15"/>
+      <c r="F41" s="27" t="s">
+        <v>17</v>
+      </c>
+      <c r="G41" s="28"/>
+    </row>
+    <row r="42" ht="19.5" customHeight="1" spans="1:7">
+      <c r="A42" s="15">
         <v>30</v>
       </c>
-      <c r="B41" s="35"/>
-      <c r="C41" s="35"/>
-      <c r="D41" s="35"/>
-      <c r="E41" s="31"/>
-      <c r="F41" s="33" t="s">
-        <v>13</v>
-      </c>
-      <c r="G41" s="34"/>
-    </row>
-    <row r="42" spans="1:7" ht="19.5" customHeight="1">
-      <c r="A42" s="31">
+      <c r="B42" s="17"/>
+      <c r="C42" s="17"/>
+      <c r="D42" s="17"/>
+      <c r="E42" s="15"/>
+      <c r="F42" s="27" t="s">
+        <v>17</v>
+      </c>
+      <c r="G42" s="28"/>
+    </row>
+    <row r="43" ht="19.5" customHeight="1" spans="1:7">
+      <c r="A43" s="15">
         <v>31</v>
       </c>
-      <c r="B42" s="35"/>
-      <c r="C42" s="35"/>
-      <c r="D42" s="35"/>
-      <c r="E42" s="31"/>
-      <c r="F42" s="33" t="s">
-        <v>13</v>
-      </c>
-      <c r="G42" s="34"/>
-    </row>
-    <row r="43" spans="1:7" ht="19.5" customHeight="1">
-      <c r="A43" s="1"/>
-      <c r="B43" s="1"/>
-      <c r="C43" s="1"/>
-    </row>
-    <row r="44" spans="1:7" ht="19.5" customHeight="1">
-      <c r="A44" s="11" t="s">
+      <c r="B43" s="17"/>
+      <c r="C43" s="17"/>
+      <c r="D43" s="17"/>
+      <c r="E43" s="15"/>
+      <c r="F43" s="27" t="s">
         <v>17</v>
       </c>
-      <c r="B44" s="12"/>
-      <c r="C44" s="2">
-        <f>SUM(C12:C43)</f>
+      <c r="G43" s="28"/>
+    </row>
+    <row r="44" ht="19.5" customHeight="1" spans="1:3">
+      <c r="A44" s="18"/>
+      <c r="B44" s="18"/>
+      <c r="C44" s="18"/>
+    </row>
+    <row r="45" ht="19.5" customHeight="1" spans="1:3">
+      <c r="A45" s="19" t="s">
+        <v>21</v>
+      </c>
+      <c r="B45" s="20"/>
+      <c r="C45" s="21">
+        <f>SUM(C13:C44)</f>
         <v>0</v>
       </c>
     </row>
-    <row r="45" spans="1:7" ht="19.5" customHeight="1"/>
-    <row r="46" spans="1:7" ht="19.5" customHeight="1"/>
-    <row r="47" spans="1:7" ht="19.5" customHeight="1">
-      <c r="C47" s="13" t="s">
-        <v>18</v>
-      </c>
-      <c r="D47" s="14"/>
-      <c r="E47" s="15"/>
-    </row>
-    <row r="48" spans="1:7" ht="57.75" customHeight="1">
-      <c r="C48" s="16"/>
-      <c r="D48" s="14"/>
-      <c r="E48" s="15"/>
-    </row>
-    <row r="49" ht="12.75" customHeight="1"/>
+    <row r="46" ht="19.5" customHeight="1"/>
+    <row r="47" ht="19.5" customHeight="1"/>
+    <row r="48" ht="57.75" customHeight="1" spans="3:5">
+      <c r="C48" s="22" t="s">
+        <v>22</v>
+      </c>
+      <c r="D48" s="23"/>
+      <c r="E48" s="29"/>
+    </row>
+    <row r="49" ht="12.75" customHeight="1" spans="3:5">
+      <c r="C49" s="24"/>
+      <c r="D49" s="23"/>
+      <c r="E49" s="29"/>
+    </row>
     <row r="50" ht="12.75" customHeight="1"/>
     <row r="51" ht="12.75" customHeight="1"/>
     <row r="52" ht="12.75" customHeight="1"/>
@@ -2463,33 +3143,38 @@
     <row r="1009" ht="15.75" customHeight="1"/>
     <row r="1010" ht="15.75" customHeight="1"/>
   </sheetData>
-  <mergeCells count="23">
-    <mergeCell ref="C48:E48"/>
+  <mergeCells count="27">
     <mergeCell ref="A1:G1"/>
     <mergeCell ref="A2:G2"/>
+    <mergeCell ref="A3:B3"/>
     <mergeCell ref="C3:G3"/>
+    <mergeCell ref="A4:B4"/>
     <mergeCell ref="C4:G4"/>
+    <mergeCell ref="A5:B5"/>
     <mergeCell ref="C5:G5"/>
+    <mergeCell ref="A6:B6"/>
     <mergeCell ref="C6:G6"/>
+    <mergeCell ref="A7:B7"/>
     <mergeCell ref="C7:G7"/>
+    <mergeCell ref="A8:B8"/>
     <mergeCell ref="C8:G8"/>
+    <mergeCell ref="A9:B9"/>
+    <mergeCell ref="C9:G9"/>
+    <mergeCell ref="A10:B10"/>
+    <mergeCell ref="C10:G10"/>
+    <mergeCell ref="J13:M13"/>
+    <mergeCell ref="J14:M14"/>
+    <mergeCell ref="J16:M16"/>
     <mergeCell ref="J17:M17"/>
     <mergeCell ref="J19:M19"/>
     <mergeCell ref="J20:M20"/>
-    <mergeCell ref="A44:B44"/>
-    <mergeCell ref="C47:E47"/>
-    <mergeCell ref="A8:B8"/>
-    <mergeCell ref="J13:M13"/>
-    <mergeCell ref="J14:M14"/>
-    <mergeCell ref="J16:M16"/>
-    <mergeCell ref="A5:B5"/>
-    <mergeCell ref="A6:B6"/>
-    <mergeCell ref="A7:B7"/>
-    <mergeCell ref="A3:B3"/>
-    <mergeCell ref="A4:B4"/>
+    <mergeCell ref="A45:B45"/>
+    <mergeCell ref="C48:E48"/>
+    <mergeCell ref="C49:E49"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0" footer="0"/>
   <pageSetup paperSize="9" scale="84" orientation="portrait"/>
+  <headerFooter/>
   <drawing r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
feat: add CNPJ field to company management and update related forms and spreadsheets
</commit_message>
<xml_diff>
--- a/src/data/model.xlsx
+++ b/src/data/model.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="3" lowestEdited="5" rupBuild="9302"/>
   <workbookPr/>
   <bookViews>
-    <workbookView windowWidth="27930" windowHeight="12495"/>
+    <workbookView windowWidth="27975" windowHeight="12495"/>
   </bookViews>
   <sheets>
     <sheet name="FREQUÊNCIA" sheetId="1" r:id="rId1"/>
@@ -42,6 +42,9 @@
       </rPr>
       <t>Profissional executante:</t>
     </r>
+  </si>
+  <si>
+    <t>Terapia:</t>
   </si>
   <si>
     <r>
@@ -174,15 +177,6 @@
     <t>Presencial</t>
   </si>
   <si>
-    <t>DIAS DE ATENDIMENTO</t>
-  </si>
-  <si>
-    <t>COMPETENCIA</t>
-  </si>
-  <si>
-    <t>HORÁRIO</t>
-  </si>
-  <si>
     <r>
       <rPr>
         <b/>
@@ -206,6 +200,12 @@
       <t>Profissional Executante (Carimbar)</t>
     </r>
   </si>
+  <si>
+    <t>DIAS DE ATENDIMENTO</t>
+  </si>
+  <si>
+    <t>COMPETENCIA</t>
+  </si>
 </sst>
 </file>
 
@@ -213,9 +213,9 @@
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="4">
     <numFmt numFmtId="176" formatCode="_-* #,##0_-;\-* #,##0_-;_-* &quot;-&quot;_-;_-@_-"/>
-    <numFmt numFmtId="177" formatCode="_-* #,##0.00_-;\-* #,##0.00_-;_-* &quot;-&quot;??_-;_-@_-"/>
+    <numFmt numFmtId="177" formatCode="_-&quot;R$&quot;\ * #,##0_-;\-&quot;R$&quot;\ * #,##0_-;_-&quot;R$&quot;\ * &quot;-&quot;_-;_-@_-"/>
     <numFmt numFmtId="178" formatCode="_-&quot;R$&quot;\ * #,##0.00_-;\-&quot;R$&quot;\ * #,##0.00_-;_-&quot;R$&quot;\ * &quot;-&quot;??_-;_-@_-"/>
-    <numFmt numFmtId="179" formatCode="_-&quot;R$&quot;\ * #,##0_-;\-&quot;R$&quot;\ * #,##0_-;_-&quot;R$&quot;\ * &quot;-&quot;_-;_-@_-"/>
+    <numFmt numFmtId="179" formatCode="_-* #,##0.00_-;\-* #,##0.00_-;_-* &quot;-&quot;??_-;_-@_-"/>
   </numFmts>
   <fonts count="33">
     <font>
@@ -296,15 +296,15 @@
       <charset val="134"/>
     </font>
     <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+    </font>
+    <font>
       <sz val="8"/>
       <color theme="1"/>
       <name val="Tahoma"/>
-      <charset val="134"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
       <charset val="134"/>
     </font>
     <font>
@@ -317,15 +317,16 @@
     </font>
     <font>
       <b/>
+      <sz val="13"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
       <sz val="11"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FFFF0000"/>
+      <color rgb="FF800080"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -354,24 +355,78 @@
     </font>
     <font>
       <sz val="11"/>
+      <color theme="0"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF9C6500"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FFFA7D00"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF3F3F76"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
       <color rgb="FF9C0006"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
-      <u/>
+      <b/>
       <sz val="11"/>
-      <color rgb="FF800080"/>
+      <color rgb="FFFFFFFF"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
+      <i/>
       <sz val="11"/>
-      <color theme="0"/>
+      <color rgb="FF7F7F7F"/>
       <name val="Calibri"/>
       <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="18"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
       <scheme val="minor"/>
     </font>
     <font>
@@ -384,73 +439,18 @@
     </font>
     <font>
       <sz val="11"/>
-      <color rgb="FF3F3F76"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
       <color rgb="FFFA7D00"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
-      <b/>
-      <sz val="13"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
       <sz val="11"/>
-      <color rgb="FFFA7D00"/>
+      <color rgb="FFFF0000"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
     </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF9C6500"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FFFFFFFF"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="18"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <i/>
-      <sz val="11"/>
-      <color rgb="FF7F7F7F"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
   </fonts>
   <fills count="41">
     <fill>
@@ -521,13 +521,127 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFEB9C"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFF2F2F2"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFCC99"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFFCC"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor rgb="FFFFC7CE"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFFFFFCC"/>
+        <fgColor theme="7" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFA5A5A5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.799981688894314"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -539,157 +653,43 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor theme="6" tint="0.799981688894314"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFF2F2F2"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFCC99"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
         <fgColor theme="6"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFEB9C"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFA5A5A5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -833,28 +833,6 @@
       <diagonal/>
     </border>
     <border>
-      <left style="thin">
-        <color theme="2" tint="-0.249977111117893"/>
-      </left>
-      <right/>
-      <top/>
-      <bottom/>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right style="thin">
-        <color rgb="FFA5A5A5"/>
-      </right>
-      <top style="thin">
-        <color rgb="FFA5A5A5"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FFA5A5A5"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
       <left style="medium">
         <color rgb="FF000000"/>
       </left>
@@ -899,6 +877,28 @@
       <diagonal/>
     </border>
     <border>
+      <left style="thin">
+        <color theme="2" tint="-0.249977111117893"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color rgb="FFA5A5A5"/>
+      </right>
+      <top style="thin">
+        <color rgb="FFA5A5A5"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FFA5A5A5"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
       <left/>
       <right style="medium">
         <color rgb="FF000000"/>
@@ -925,20 +925,24 @@
     <border>
       <left/>
       <right/>
-      <top style="thin">
-        <color theme="4"/>
-      </top>
-      <bottom style="double">
+      <top/>
+      <bottom style="medium">
         <color theme="4"/>
       </bottom>
       <diagonal/>
     </border>
     <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="medium">
-        <color theme="4"/>
+      <left style="thin">
+        <color rgb="FF7F7F7F"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF7F7F7F"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF7F7F7F"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF7F7F7F"/>
       </bottom>
       <diagonal/>
     </border>
@@ -958,50 +962,13 @@
       <diagonal/>
     </border>
     <border>
-      <left style="thin">
-        <color rgb="FF3F3F3F"/>
-      </left>
-      <right style="thin">
-        <color rgb="FF3F3F3F"/>
-      </right>
-      <top style="thin">
-        <color rgb="FF3F3F3F"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FF3F3F3F"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color rgb="FF7F7F7F"/>
-      </left>
-      <right style="thin">
-        <color rgb="FF7F7F7F"/>
-      </right>
-      <top style="thin">
-        <color rgb="FF7F7F7F"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FF7F7F7F"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
       <left/>
       <right/>
-      <top/>
+      <top style="thin">
+        <color theme="4"/>
+      </top>
       <bottom style="double">
-        <color rgb="FFFF8001"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="medium">
-        <color theme="4" tint="0.499984740745262"/>
+        <color theme="4"/>
       </bottom>
       <diagonal/>
     </border>
@@ -1020,145 +987,178 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color theme="4" tint="0.499984740745262"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FF3F3F3F"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF3F3F3F"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF3F3F3F"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF3F3F3F"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="double">
+        <color rgb="FFFF8001"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="49">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="22" fillId="40" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="20" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="17" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="22" fillId="35" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="22" fillId="38" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="22" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="22" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="20" fillId="36" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="38" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="37" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="35" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="34" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="31" fillId="0" borderId="26" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="40" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="26" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="25" fillId="0" borderId="22" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="30" fillId="14" borderId="25" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="178" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="17" fillId="39" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="22" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="25" fillId="0" borderId="24" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="22" fillId="34" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="22" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="22" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="22" fillId="33" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="29" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="22" fillId="37" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="0" fillId="16" borderId="21" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="24" fillId="15" borderId="20" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="23" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="14" borderId="20" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="23" fillId="0" borderId="24" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="28" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="19" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="176" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="177" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="32" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="15" fillId="0" borderId="19" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="23" fillId="16" borderId="22" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="178" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="13" borderId="21" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="24" fillId="24" borderId="23" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="28" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="27" fillId="16" borderId="23" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="28" fillId="0" borderId="25" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="32" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="20" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="176" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="31" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
     <xf numFmtId="179" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="26" fillId="0" borderId="20" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="177" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="30" fillId="36" borderId="26" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="22" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="27" fillId="27" borderId="23" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="33" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="9" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
@@ -1236,28 +1236,28 @@
     <xf numFmtId="0" fontId="10" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="12" fillId="8" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="12" fillId="9" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="9" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="10" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="13" fillId="8" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="13" fillId="9" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="9" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="13" fillId="9" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="12" fillId="9" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1"/>
@@ -1556,14 +1556,16 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
-  <sheetPr/>
-  <dimension ref="A1:M1010"/>
+  <sheetPr>
+    <pageSetUpPr fitToPage="1"/>
+  </sheetPr>
+  <dimension ref="A1:H1010"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H11" sqref="H11"/>
+    <sheetView tabSelected="1" topLeftCell="A34" workbookViewId="0">
+      <selection activeCell="G58" sqref="G58"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="14.4416666666667" defaultRowHeight="15" customHeight="1"/>
+  <sheetFormatPr defaultColWidth="14.4416666666667" defaultRowHeight="15" customHeight="1" outlineLevelCol="7"/>
   <cols>
     <col min="1" max="1" width="16" customWidth="1"/>
     <col min="2" max="2" width="15.6666666666667" customWidth="1"/>
@@ -1587,7 +1589,7 @@
       <c r="E1" s="2"/>
       <c r="F1" s="2"/>
       <c r="G1" s="2"/>
-      <c r="H1" s="25"/>
+      <c r="H1" s="30"/>
     </row>
     <row r="2" ht="21.75" customHeight="1" spans="1:8">
       <c r="A2" s="3" t="s">
@@ -1599,7 +1601,7 @@
       <c r="E2" s="4"/>
       <c r="F2" s="4"/>
       <c r="G2" s="4"/>
-      <c r="H2" s="25"/>
+      <c r="H2" s="30"/>
     </row>
     <row r="3" ht="16.5" customHeight="1" spans="1:8">
       <c r="A3" s="5" t="s">
@@ -1611,7 +1613,7 @@
       <c r="E3" s="6"/>
       <c r="F3" s="6"/>
       <c r="G3" s="6"/>
-      <c r="H3" s="26"/>
+      <c r="H3" s="31"/>
     </row>
     <row r="4" ht="16.5" customHeight="1" spans="1:8">
       <c r="A4" s="5" t="s">
@@ -1623,43 +1625,43 @@
       <c r="E4" s="6"/>
       <c r="F4" s="6"/>
       <c r="G4" s="6"/>
-      <c r="H4" s="26"/>
+      <c r="H4" s="31"/>
     </row>
     <row r="5" ht="16.5" customHeight="1" spans="1:8">
-      <c r="A5" s="8" t="s">
+      <c r="A5" s="5" t="s">
         <v>4</v>
       </c>
       <c r="B5" s="7"/>
-      <c r="C5" s="9"/>
-      <c r="D5" s="9"/>
-      <c r="E5" s="9"/>
-      <c r="F5" s="9"/>
-      <c r="G5" s="9"/>
-      <c r="H5" s="26"/>
+      <c r="C5" s="6"/>
+      <c r="D5" s="6"/>
+      <c r="E5" s="6"/>
+      <c r="F5" s="6"/>
+      <c r="G5" s="6"/>
+      <c r="H5" s="31"/>
     </row>
     <row r="6" ht="16.5" customHeight="1" spans="1:8">
-      <c r="A6" s="5" t="s">
+      <c r="A6" s="8" t="s">
         <v>5</v>
       </c>
       <c r="B6" s="7"/>
-      <c r="C6" s="10"/>
-      <c r="D6" s="10"/>
-      <c r="E6" s="10"/>
-      <c r="F6" s="10"/>
-      <c r="G6" s="10"/>
-      <c r="H6" s="26"/>
+      <c r="C6" s="9"/>
+      <c r="D6" s="9"/>
+      <c r="E6" s="9"/>
+      <c r="F6" s="9"/>
+      <c r="G6" s="9"/>
+      <c r="H6" s="31"/>
     </row>
     <row r="7" ht="16.5" customHeight="1" spans="1:8">
       <c r="A7" s="5" t="s">
         <v>6</v>
       </c>
       <c r="B7" s="7"/>
-      <c r="C7" s="6"/>
-      <c r="D7" s="6"/>
-      <c r="E7" s="6"/>
-      <c r="F7" s="6"/>
-      <c r="G7" s="6"/>
-      <c r="H7" s="26"/>
+      <c r="C7" s="10"/>
+      <c r="D7" s="10"/>
+      <c r="E7" s="10"/>
+      <c r="F7" s="10"/>
+      <c r="G7" s="10"/>
+      <c r="H7" s="31"/>
     </row>
     <row r="8" ht="16.5" customHeight="1" spans="1:8">
       <c r="A8" s="5" t="s">
@@ -1671,13 +1673,13 @@
       <c r="E8" s="6"/>
       <c r="F8" s="6"/>
       <c r="G8" s="6"/>
-      <c r="H8" s="26"/>
+      <c r="H8" s="31"/>
     </row>
     <row r="9" ht="12.75" customHeight="1" spans="1:7">
-      <c r="A9" s="11" t="s">
+      <c r="A9" s="5" t="s">
         <v>8</v>
       </c>
-      <c r="B9" s="12"/>
+      <c r="B9" s="7"/>
       <c r="C9" s="6"/>
       <c r="D9" s="6"/>
       <c r="E9" s="6"/>
@@ -1685,510 +1687,514 @@
       <c r="G9" s="6"/>
     </row>
     <row r="10" ht="12.75" customHeight="1" spans="1:7">
-      <c r="A10" s="13" t="s">
+      <c r="A10" s="11" t="s">
         <v>9</v>
       </c>
-      <c r="B10" s="13"/>
+      <c r="B10" s="12"/>
       <c r="C10" s="6"/>
       <c r="D10" s="6"/>
       <c r="E10" s="6"/>
       <c r="F10" s="6"/>
       <c r="G10" s="6"/>
     </row>
-    <row r="11" ht="19.5" customHeight="1"/>
-    <row r="12" ht="19.5" customHeight="1" spans="1:7">
-      <c r="A12" s="14" t="s">
+    <row r="11" ht="19.5" customHeight="1" spans="1:7">
+      <c r="A11" s="13" t="s">
         <v>10</v>
       </c>
-      <c r="B12" s="14" t="s">
+      <c r="B11" s="13"/>
+      <c r="C11" s="6"/>
+      <c r="D11" s="6"/>
+      <c r="E11" s="6"/>
+      <c r="F11" s="6"/>
+      <c r="G11" s="6"/>
+    </row>
+    <row r="12" ht="19.5" customHeight="1"/>
+    <row r="13" ht="19.5" customHeight="1" spans="1:7">
+      <c r="A13" s="14" t="s">
         <v>11</v>
       </c>
-      <c r="C12" s="14" t="s">
+      <c r="B13" s="14" t="s">
         <v>12</v>
       </c>
-      <c r="D12" s="14" t="s">
+      <c r="C13" s="14" t="s">
         <v>13</v>
       </c>
-      <c r="E12" s="14" t="s">
+      <c r="D13" s="14" t="s">
         <v>14</v>
       </c>
-      <c r="F12" s="14" t="s">
+      <c r="E13" s="14" t="s">
         <v>15</v>
       </c>
-      <c r="G12" s="14" t="s">
+      <c r="F13" s="14" t="s">
         <v>16</v>
       </c>
-    </row>
-    <row r="13" ht="19.5" customHeight="1" spans="1:13">
-      <c r="A13" s="15">
+      <c r="G13" s="14" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="14" ht="19.5" customHeight="1" spans="1:7">
+      <c r="A14" s="15">
         <v>1</v>
-      </c>
-      <c r="B13" s="16"/>
-      <c r="C13" s="16"/>
-      <c r="D13" s="16"/>
-      <c r="E13" s="15"/>
-      <c r="F13" s="27" t="s">
-        <v>17</v>
-      </c>
-      <c r="G13" s="28"/>
-      <c r="J13" s="30" t="s">
-        <v>18</v>
-      </c>
-      <c r="K13" s="31"/>
-      <c r="L13" s="31"/>
-      <c r="M13" s="35"/>
-    </row>
-    <row r="14" ht="19.5" customHeight="1" spans="1:13">
-      <c r="A14" s="15">
-        <v>2</v>
       </c>
       <c r="B14" s="16"/>
       <c r="C14" s="16"/>
       <c r="D14" s="16"/>
       <c r="E14" s="15"/>
-      <c r="F14" s="27" t="s">
-        <v>17</v>
-      </c>
-      <c r="G14" s="28"/>
-      <c r="J14" s="32"/>
-      <c r="K14" s="33"/>
-      <c r="L14" s="33"/>
-      <c r="M14" s="36"/>
+      <c r="F14" s="32" t="s">
+        <v>18</v>
+      </c>
+      <c r="G14" s="33"/>
     </row>
     <row r="15" ht="19.5" customHeight="1" spans="1:7">
       <c r="A15" s="15">
+        <v>2</v>
+      </c>
+      <c r="B15" s="16"/>
+      <c r="C15" s="16"/>
+      <c r="D15" s="16"/>
+      <c r="E15" s="15"/>
+      <c r="F15" s="32" t="s">
+        <v>18</v>
+      </c>
+      <c r="G15" s="33"/>
+    </row>
+    <row r="16" ht="19.5" customHeight="1" spans="1:7">
+      <c r="A16" s="15">
         <v>3</v>
-      </c>
-      <c r="B15" s="17"/>
-      <c r="C15" s="17"/>
-      <c r="D15" s="17"/>
-      <c r="E15" s="15"/>
-      <c r="F15" s="27" t="s">
-        <v>17</v>
-      </c>
-      <c r="G15" s="28"/>
-    </row>
-    <row r="16" ht="19.5" customHeight="1" spans="1:13">
-      <c r="A16" s="15">
-        <v>4</v>
       </c>
       <c r="B16" s="17"/>
       <c r="C16" s="17"/>
       <c r="D16" s="17"/>
       <c r="E16" s="15"/>
-      <c r="F16" s="27" t="s">
-        <v>17</v>
-      </c>
-      <c r="G16" s="28"/>
-      <c r="J16" s="30" t="s">
-        <v>19</v>
-      </c>
-      <c r="K16" s="31"/>
-      <c r="L16" s="31"/>
-      <c r="M16" s="35"/>
-    </row>
-    <row r="17" ht="19.5" customHeight="1" spans="1:13">
+      <c r="F16" s="32" t="s">
+        <v>18</v>
+      </c>
+      <c r="G16" s="33"/>
+    </row>
+    <row r="17" ht="19.5" customHeight="1" spans="1:7">
       <c r="A17" s="15">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="B17" s="17"/>
       <c r="C17" s="17"/>
       <c r="D17" s="17"/>
       <c r="E17" s="15"/>
-      <c r="F17" s="27" t="s">
-        <v>17</v>
-      </c>
-      <c r="G17" s="28"/>
-      <c r="J17" s="32"/>
-      <c r="K17" s="34"/>
-      <c r="L17" s="34"/>
-      <c r="M17" s="37"/>
+      <c r="F17" s="32" t="s">
+        <v>18</v>
+      </c>
+      <c r="G17" s="33"/>
     </row>
     <row r="18" ht="19.5" customHeight="1" spans="1:7">
       <c r="A18" s="15">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="B18" s="17"/>
       <c r="C18" s="17"/>
       <c r="D18" s="17"/>
       <c r="E18" s="15"/>
-      <c r="F18" s="27" t="s">
-        <v>17</v>
-      </c>
-      <c r="G18" s="28"/>
-    </row>
-    <row r="19" ht="19.5" customHeight="1" spans="1:13">
+      <c r="F18" s="32" t="s">
+        <v>18</v>
+      </c>
+      <c r="G18" s="33"/>
+    </row>
+    <row r="19" ht="19.5" customHeight="1" spans="1:7">
       <c r="A19" s="15">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="B19" s="17"/>
       <c r="C19" s="17"/>
       <c r="D19" s="17"/>
       <c r="E19" s="15"/>
-      <c r="F19" s="27" t="s">
-        <v>17</v>
-      </c>
-      <c r="G19" s="28"/>
-      <c r="J19" s="30" t="s">
-        <v>20</v>
-      </c>
-      <c r="K19" s="31"/>
-      <c r="L19" s="31"/>
-      <c r="M19" s="35"/>
-    </row>
-    <row r="20" ht="19.5" customHeight="1" spans="1:13">
+      <c r="F19" s="32" t="s">
+        <v>18</v>
+      </c>
+      <c r="G19" s="33"/>
+    </row>
+    <row r="20" ht="19.5" customHeight="1" spans="1:7">
       <c r="A20" s="15">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="B20" s="17"/>
       <c r="C20" s="17"/>
       <c r="D20" s="17"/>
       <c r="E20" s="15"/>
-      <c r="F20" s="27" t="s">
-        <v>17</v>
-      </c>
-      <c r="G20" s="28"/>
-      <c r="J20" s="32"/>
-      <c r="K20" s="33"/>
-      <c r="L20" s="33"/>
-      <c r="M20" s="36"/>
+      <c r="F20" s="32" t="s">
+        <v>18</v>
+      </c>
+      <c r="G20" s="33"/>
     </row>
     <row r="21" ht="19.5" customHeight="1" spans="1:7">
       <c r="A21" s="15">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="B21" s="17"/>
       <c r="C21" s="17"/>
       <c r="D21" s="17"/>
       <c r="E21" s="15"/>
-      <c r="F21" s="27" t="s">
-        <v>17</v>
-      </c>
-      <c r="G21" s="28"/>
+      <c r="F21" s="32" t="s">
+        <v>18</v>
+      </c>
+      <c r="G21" s="33"/>
     </row>
     <row r="22" ht="19.5" customHeight="1" spans="1:7">
       <c r="A22" s="15">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="B22" s="17"/>
       <c r="C22" s="17"/>
       <c r="D22" s="17"/>
       <c r="E22" s="15"/>
-      <c r="F22" s="27" t="s">
-        <v>17</v>
-      </c>
-      <c r="G22" s="28"/>
+      <c r="F22" s="32" t="s">
+        <v>18</v>
+      </c>
+      <c r="G22" s="33"/>
     </row>
     <row r="23" ht="19.5" customHeight="1" spans="1:7">
       <c r="A23" s="15">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="B23" s="17"/>
       <c r="C23" s="17"/>
       <c r="D23" s="17"/>
       <c r="E23" s="15"/>
-      <c r="F23" s="27" t="s">
-        <v>17</v>
-      </c>
-      <c r="G23" s="28"/>
+      <c r="F23" s="32" t="s">
+        <v>18</v>
+      </c>
+      <c r="G23" s="33"/>
     </row>
     <row r="24" ht="19.5" customHeight="1" spans="1:7">
       <c r="A24" s="15">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="B24" s="17"/>
       <c r="C24" s="17"/>
       <c r="D24" s="17"/>
       <c r="E24" s="15"/>
-      <c r="F24" s="27" t="s">
-        <v>17</v>
-      </c>
-      <c r="G24" s="28"/>
+      <c r="F24" s="32" t="s">
+        <v>18</v>
+      </c>
+      <c r="G24" s="33"/>
     </row>
     <row r="25" ht="19.5" customHeight="1" spans="1:7">
       <c r="A25" s="15">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="B25" s="17"/>
       <c r="C25" s="17"/>
       <c r="D25" s="17"/>
       <c r="E25" s="15"/>
-      <c r="F25" s="27" t="s">
-        <v>17</v>
-      </c>
-      <c r="G25" s="28"/>
+      <c r="F25" s="32" t="s">
+        <v>18</v>
+      </c>
+      <c r="G25" s="33"/>
     </row>
     <row r="26" ht="19.5" customHeight="1" spans="1:7">
       <c r="A26" s="15">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="B26" s="17"/>
       <c r="C26" s="17"/>
       <c r="D26" s="17"/>
       <c r="E26" s="15"/>
-      <c r="F26" s="27" t="s">
-        <v>17</v>
-      </c>
-      <c r="G26" s="28"/>
+      <c r="F26" s="32" t="s">
+        <v>18</v>
+      </c>
+      <c r="G26" s="33"/>
     </row>
     <row r="27" ht="19.5" customHeight="1" spans="1:7">
       <c r="A27" s="15">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="B27" s="17"/>
       <c r="C27" s="17"/>
       <c r="D27" s="17"/>
       <c r="E27" s="15"/>
-      <c r="F27" s="27" t="s">
-        <v>17</v>
-      </c>
-      <c r="G27" s="28"/>
+      <c r="F27" s="32" t="s">
+        <v>18</v>
+      </c>
+      <c r="G27" s="33"/>
     </row>
     <row r="28" ht="19.5" customHeight="1" spans="1:7">
       <c r="A28" s="15">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="B28" s="17"/>
       <c r="C28" s="17"/>
       <c r="D28" s="17"/>
       <c r="E28" s="15"/>
-      <c r="F28" s="27" t="s">
-        <v>17</v>
-      </c>
-      <c r="G28" s="28"/>
+      <c r="F28" s="32" t="s">
+        <v>18</v>
+      </c>
+      <c r="G28" s="33"/>
     </row>
     <row r="29" ht="19.5" customHeight="1" spans="1:7">
       <c r="A29" s="15">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="B29" s="17"/>
       <c r="C29" s="17"/>
       <c r="D29" s="17"/>
       <c r="E29" s="15"/>
-      <c r="F29" s="27" t="s">
-        <v>17</v>
-      </c>
-      <c r="G29" s="28"/>
+      <c r="F29" s="32" t="s">
+        <v>18</v>
+      </c>
+      <c r="G29" s="33"/>
     </row>
     <row r="30" ht="19.5" customHeight="1" spans="1:7">
       <c r="A30" s="15">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="B30" s="17"/>
       <c r="C30" s="17"/>
       <c r="D30" s="17"/>
       <c r="E30" s="15"/>
-      <c r="F30" s="27" t="s">
-        <v>17</v>
-      </c>
-      <c r="G30" s="28"/>
+      <c r="F30" s="32" t="s">
+        <v>18</v>
+      </c>
+      <c r="G30" s="33"/>
     </row>
     <row r="31" ht="19.5" customHeight="1" spans="1:7">
       <c r="A31" s="15">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="B31" s="17"/>
       <c r="C31" s="17"/>
       <c r="D31" s="17"/>
       <c r="E31" s="15"/>
-      <c r="F31" s="27" t="s">
-        <v>17</v>
-      </c>
-      <c r="G31" s="28"/>
+      <c r="F31" s="32" t="s">
+        <v>18</v>
+      </c>
+      <c r="G31" s="33"/>
     </row>
     <row r="32" ht="19.5" customHeight="1" spans="1:7">
       <c r="A32" s="15">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="B32" s="17"/>
       <c r="C32" s="17"/>
       <c r="D32" s="17"/>
       <c r="E32" s="15"/>
-      <c r="F32" s="27" t="s">
-        <v>17</v>
-      </c>
-      <c r="G32" s="28"/>
+      <c r="F32" s="32" t="s">
+        <v>18</v>
+      </c>
+      <c r="G32" s="33"/>
     </row>
     <row r="33" ht="19.5" customHeight="1" spans="1:7">
       <c r="A33" s="15">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="B33" s="17"/>
       <c r="C33" s="17"/>
       <c r="D33" s="17"/>
       <c r="E33" s="15"/>
-      <c r="F33" s="27" t="s">
-        <v>17</v>
-      </c>
-      <c r="G33" s="28"/>
+      <c r="F33" s="32" t="s">
+        <v>18</v>
+      </c>
+      <c r="G33" s="33"/>
     </row>
     <row r="34" ht="19.5" customHeight="1" spans="1:7">
       <c r="A34" s="15">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="B34" s="17"/>
       <c r="C34" s="17"/>
       <c r="D34" s="17"/>
       <c r="E34" s="15"/>
-      <c r="F34" s="27" t="s">
-        <v>17</v>
-      </c>
-      <c r="G34" s="28"/>
+      <c r="F34" s="32" t="s">
+        <v>18</v>
+      </c>
+      <c r="G34" s="33"/>
     </row>
     <row r="35" ht="19.5" customHeight="1" spans="1:7">
       <c r="A35" s="15">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="B35" s="17"/>
       <c r="C35" s="17"/>
       <c r="D35" s="17"/>
       <c r="E35" s="15"/>
-      <c r="F35" s="27" t="s">
-        <v>17</v>
-      </c>
-      <c r="G35" s="28"/>
+      <c r="F35" s="32" t="s">
+        <v>18</v>
+      </c>
+      <c r="G35" s="33"/>
     </row>
     <row r="36" ht="19.5" customHeight="1" spans="1:7">
       <c r="A36" s="15">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="B36" s="17"/>
       <c r="C36" s="17"/>
       <c r="D36" s="17"/>
       <c r="E36" s="15"/>
-      <c r="F36" s="27" t="s">
-        <v>17</v>
-      </c>
-      <c r="G36" s="28"/>
+      <c r="F36" s="32" t="s">
+        <v>18</v>
+      </c>
+      <c r="G36" s="33"/>
     </row>
     <row r="37" ht="19.5" customHeight="1" spans="1:7">
       <c r="A37" s="15">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="B37" s="17"/>
       <c r="C37" s="17"/>
       <c r="D37" s="17"/>
       <c r="E37" s="15"/>
-      <c r="F37" s="27" t="s">
-        <v>17</v>
-      </c>
-      <c r="G37" s="28"/>
+      <c r="F37" s="32" t="s">
+        <v>18</v>
+      </c>
+      <c r="G37" s="33"/>
     </row>
     <row r="38" ht="19.5" customHeight="1" spans="1:7">
       <c r="A38" s="15">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="B38" s="17"/>
       <c r="C38" s="17"/>
       <c r="D38" s="17"/>
       <c r="E38" s="15"/>
-      <c r="F38" s="27" t="s">
-        <v>17</v>
-      </c>
-      <c r="G38" s="28"/>
+      <c r="F38" s="32" t="s">
+        <v>18</v>
+      </c>
+      <c r="G38" s="33"/>
     </row>
     <row r="39" ht="19.5" customHeight="1" spans="1:7">
       <c r="A39" s="15">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="B39" s="17"/>
       <c r="C39" s="17"/>
       <c r="D39" s="17"/>
       <c r="E39" s="15"/>
-      <c r="F39" s="27" t="s">
-        <v>17</v>
-      </c>
-      <c r="G39" s="28"/>
+      <c r="F39" s="32" t="s">
+        <v>18</v>
+      </c>
+      <c r="G39" s="33"/>
     </row>
     <row r="40" ht="19.5" customHeight="1" spans="1:7">
       <c r="A40" s="15">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="B40" s="17"/>
       <c r="C40" s="17"/>
       <c r="D40" s="17"/>
       <c r="E40" s="15"/>
-      <c r="F40" s="27" t="s">
-        <v>17</v>
-      </c>
-      <c r="G40" s="28"/>
+      <c r="F40" s="32" t="s">
+        <v>18</v>
+      </c>
+      <c r="G40" s="33"/>
     </row>
     <row r="41" ht="19.5" customHeight="1" spans="1:7">
       <c r="A41" s="15">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="B41" s="17"/>
       <c r="C41" s="17"/>
       <c r="D41" s="17"/>
       <c r="E41" s="15"/>
-      <c r="F41" s="27" t="s">
-        <v>17</v>
-      </c>
-      <c r="G41" s="28"/>
+      <c r="F41" s="32" t="s">
+        <v>18</v>
+      </c>
+      <c r="G41" s="33"/>
     </row>
     <row r="42" ht="19.5" customHeight="1" spans="1:7">
       <c r="A42" s="15">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="B42" s="17"/>
       <c r="C42" s="17"/>
       <c r="D42" s="17"/>
       <c r="E42" s="15"/>
-      <c r="F42" s="27" t="s">
-        <v>17</v>
-      </c>
-      <c r="G42" s="28"/>
+      <c r="F42" s="32" t="s">
+        <v>18</v>
+      </c>
+      <c r="G42" s="33"/>
     </row>
     <row r="43" ht="19.5" customHeight="1" spans="1:7">
       <c r="A43" s="15">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="B43" s="17"/>
       <c r="C43" s="17"/>
       <c r="D43" s="17"/>
       <c r="E43" s="15"/>
-      <c r="F43" s="27" t="s">
-        <v>17</v>
-      </c>
-      <c r="G43" s="28"/>
-    </row>
-    <row r="44" ht="19.5" customHeight="1" spans="1:3">
-      <c r="A44" s="18"/>
-      <c r="B44" s="18"/>
-      <c r="C44" s="18"/>
+      <c r="F43" s="32" t="s">
+        <v>18</v>
+      </c>
+      <c r="G43" s="33"/>
+    </row>
+    <row r="44" ht="19.5" customHeight="1" spans="1:7">
+      <c r="A44" s="15">
+        <v>31</v>
+      </c>
+      <c r="B44" s="17"/>
+      <c r="C44" s="17"/>
+      <c r="D44" s="17"/>
+      <c r="E44" s="15"/>
+      <c r="F44" s="32" t="s">
+        <v>18</v>
+      </c>
+      <c r="G44" s="33"/>
     </row>
     <row r="45" ht="19.5" customHeight="1" spans="1:3">
-      <c r="A45" s="19" t="s">
-        <v>21</v>
-      </c>
-      <c r="B45" s="20"/>
-      <c r="C45" s="21">
-        <f>SUM(C13:C44)</f>
+      <c r="A45" s="18"/>
+      <c r="B45" s="18"/>
+      <c r="C45" s="18"/>
+    </row>
+    <row r="46" ht="19.5" customHeight="1" spans="1:3">
+      <c r="A46" s="19" t="s">
+        <v>19</v>
+      </c>
+      <c r="B46" s="20"/>
+      <c r="C46" s="21">
+        <f>SUM(C14:C45)</f>
         <v>0</v>
       </c>
     </row>
-    <row r="46" ht="19.5" customHeight="1"/>
     <row r="47" ht="19.5" customHeight="1"/>
-    <row r="48" ht="57.75" customHeight="1" spans="3:5">
-      <c r="C48" s="22" t="s">
-        <v>22</v>
-      </c>
-      <c r="D48" s="23"/>
-      <c r="E48" s="29"/>
-    </row>
+    <row r="48" ht="57.75" customHeight="1"/>
     <row r="49" ht="12.75" customHeight="1" spans="3:5">
-      <c r="C49" s="24"/>
+      <c r="C49" s="22" t="s">
+        <v>20</v>
+      </c>
       <c r="D49" s="23"/>
-      <c r="E49" s="29"/>
-    </row>
-    <row r="50" ht="12.75" customHeight="1"/>
+      <c r="E49" s="34"/>
+    </row>
+    <row r="50" ht="12.75" customHeight="1" spans="3:5">
+      <c r="C50" s="24"/>
+      <c r="D50" s="23"/>
+      <c r="E50" s="34"/>
+    </row>
     <row r="51" ht="12.75" customHeight="1"/>
     <row r="52" ht="12.75" customHeight="1"/>
-    <row r="53" ht="12.75" customHeight="1"/>
-    <row r="54" ht="12.75" customHeight="1"/>
+    <row r="53" ht="12.75" customHeight="1" spans="3:6">
+      <c r="C53" s="25" t="s">
+        <v>21</v>
+      </c>
+      <c r="D53" s="26"/>
+      <c r="E53" s="26"/>
+      <c r="F53" s="35"/>
+    </row>
+    <row r="54" ht="12.75" customHeight="1" spans="3:6">
+      <c r="C54" s="27"/>
+      <c r="D54" s="28"/>
+      <c r="E54" s="28"/>
+      <c r="F54" s="36"/>
+    </row>
     <row r="55" ht="12.75" customHeight="1"/>
-    <row r="56" ht="12.75" customHeight="1"/>
-    <row r="57" ht="12.75" customHeight="1"/>
+    <row r="56" ht="12.75" customHeight="1" spans="3:6">
+      <c r="C56" s="25" t="s">
+        <v>22</v>
+      </c>
+      <c r="D56" s="26"/>
+      <c r="E56" s="26"/>
+      <c r="F56" s="35"/>
+    </row>
+    <row r="57" ht="12.75" customHeight="1" spans="3:6">
+      <c r="C57" s="27"/>
+      <c r="D57" s="29"/>
+      <c r="E57" s="29"/>
+      <c r="F57" s="37"/>
+    </row>
     <row r="58" ht="12.75" customHeight="1"/>
     <row r="59" ht="12.75" customHeight="1"/>
     <row r="60" ht="12.75" customHeight="1"/>
@@ -3162,18 +3168,18 @@
     <mergeCell ref="C9:G9"/>
     <mergeCell ref="A10:B10"/>
     <mergeCell ref="C10:G10"/>
-    <mergeCell ref="J13:M13"/>
-    <mergeCell ref="J14:M14"/>
-    <mergeCell ref="J16:M16"/>
-    <mergeCell ref="J17:M17"/>
-    <mergeCell ref="J19:M19"/>
-    <mergeCell ref="J20:M20"/>
-    <mergeCell ref="A45:B45"/>
-    <mergeCell ref="C48:E48"/>
+    <mergeCell ref="A11:B11"/>
+    <mergeCell ref="C11:G11"/>
+    <mergeCell ref="A46:B46"/>
     <mergeCell ref="C49:E49"/>
+    <mergeCell ref="C50:E50"/>
+    <mergeCell ref="C53:F53"/>
+    <mergeCell ref="C54:F54"/>
+    <mergeCell ref="C56:F56"/>
+    <mergeCell ref="C57:F57"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0" footer="0"/>
-  <pageSetup paperSize="9" scale="84" orientation="portrait"/>
+  <pageSetup paperSize="9" scale="56" orientation="portrait"/>
   <headerFooter/>
   <drawing r:id="rId1"/>
 </worksheet>

</xml_diff>

<commit_message>
refactor: update layout and styling for WeekdaySessionSelector component; adjust session total cell in ExcelService
</commit_message>
<xml_diff>
--- a/src/data/model.xlsx
+++ b/src/data/model.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="3" lowestEdited="5" rupBuild="9302"/>
   <workbookPr/>
   <bookViews>
-    <workbookView windowWidth="27975" windowHeight="12495"/>
+    <workbookView windowWidth="27930" windowHeight="12495"/>
   </bookViews>
   <sheets>
     <sheet name="FREQUÊNCIA" sheetId="1" r:id="rId1"/>
@@ -212,10 +212,10 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="4">
-    <numFmt numFmtId="176" formatCode="_-* #,##0_-;\-* #,##0_-;_-* &quot;-&quot;_-;_-@_-"/>
-    <numFmt numFmtId="177" formatCode="_-&quot;R$&quot;\ * #,##0_-;\-&quot;R$&quot;\ * #,##0_-;_-&quot;R$&quot;\ * &quot;-&quot;_-;_-@_-"/>
-    <numFmt numFmtId="178" formatCode="_-&quot;R$&quot;\ * #,##0.00_-;\-&quot;R$&quot;\ * #,##0.00_-;_-&quot;R$&quot;\ * &quot;-&quot;??_-;_-@_-"/>
-    <numFmt numFmtId="179" formatCode="_-* #,##0.00_-;\-* #,##0.00_-;_-* &quot;-&quot;??_-;_-@_-"/>
+    <numFmt numFmtId="176" formatCode="_-* #,##0.00_-;\-* #,##0.00_-;_-* &quot;-&quot;??_-;_-@_-"/>
+    <numFmt numFmtId="177" formatCode="_-* #,##0_-;\-* #,##0_-;_-* &quot;-&quot;_-;_-@_-"/>
+    <numFmt numFmtId="178" formatCode="_-&quot;R$&quot;\ * #,##0_-;\-&quot;R$&quot;\ * #,##0_-;_-&quot;R$&quot;\ * &quot;-&quot;_-;_-@_-"/>
+    <numFmt numFmtId="179" formatCode="_-&quot;R$&quot;\ * #,##0.00_-;\-&quot;R$&quot;\ * #,##0.00_-;_-&quot;R$&quot;\ * &quot;-&quot;??_-;_-@_-"/>
   </numFmts>
   <fonts count="33">
     <font>
@@ -289,6 +289,18 @@
       <charset val="134"/>
     </font>
     <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+    </font>
+    <font>
+      <sz val="8"/>
+      <color theme="1"/>
+      <name val="Tahoma"/>
+      <charset val="134"/>
+    </font>
+    <font>
       <b/>
       <sz val="8"/>
       <color rgb="FF000000"/>
@@ -296,16 +308,126 @@
       <charset val="134"/>
     </font>
     <font>
+      <u/>
+      <sz val="11"/>
+      <color rgb="FF800080"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="0"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FFFA7D00"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="18"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
       <charset val="134"/>
-    </font>
-    <font>
-      <sz val="8"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="15"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <i/>
+      <sz val="11"/>
+      <color rgb="FF7F7F7F"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FFFFFFFF"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF006100"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF3F3F76"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="13"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FF3F3F3F"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
       <color theme="1"/>
-      <name val="Tahoma"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
       <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF9C0006"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF9C6500"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
     </font>
     <font>
       <u/>
@@ -316,59 +438,6 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <b/>
-      <sz val="13"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <u/>
-      <sz val="11"/>
-      <color rgb="FF800080"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="15"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF006100"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color theme="0"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF9C6500"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
       <sz val="11"/>
       <color rgb="FFFA7D00"/>
       <name val="Calibri"/>
@@ -376,75 +445,6 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <b/>
-      <sz val="11"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF3F3F76"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF9C0006"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FFFFFFFF"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <i/>
-      <sz val="11"/>
-      <color rgb="FF7F7F7F"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="18"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FF3F3F3F"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FFFA7D00"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
       <sz val="11"/>
       <color rgb="FFFF0000"/>
       <name val="Calibri"/>
@@ -509,187 +509,187 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFF2F2F2"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor theme="9" tint="0.799981688894314"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor theme="6"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFA5A5A5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor rgb="FFC6EFCE"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor rgb="FFFFCC99"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFFCC"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFC7CE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFEB9C"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor theme="9" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFFFEB9C"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFF2F2F2"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFCC99"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFFFCC"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
         <fgColor theme="9" tint="0.599993896298105"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFC7CE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
         <fgColor theme="7"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFA5A5A5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
         <fgColor theme="8" tint="0.599993896298105"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="9"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6"/>
+        <fgColor theme="8" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -795,21 +795,6 @@
     </border>
     <border>
       <left style="thin">
-        <color rgb="FFADAAAA"/>
-      </left>
-      <right style="thin">
-        <color rgb="FFA6A6A6"/>
-      </right>
-      <top style="thin">
-        <color rgb="FFA6A6A6"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FFADAAAA"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
         <color rgb="FFA5A5A5"/>
       </left>
       <right/>
@@ -886,6 +871,21 @@
       <diagonal/>
     </border>
     <border>
+      <left style="thin">
+        <color rgb="FFADAAAA"/>
+      </left>
+      <right style="thin">
+        <color rgb="FFA6A6A6"/>
+      </right>
+      <top style="thin">
+        <color rgb="FFA6A6A6"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FFADAAAA"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
       <left/>
       <right style="thin">
         <color rgb="FFA5A5A5"/>
@@ -923,15 +923,6 @@
       <diagonal/>
     </border>
     <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="medium">
-        <color theme="4"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
       <left style="thin">
         <color rgb="FF7F7F7F"/>
       </left>
@@ -947,27 +938,10 @@
       <diagonal/>
     </border>
     <border>
-      <left style="thin">
-        <color rgb="FFB2B2B2"/>
-      </left>
-      <right style="thin">
-        <color rgb="FFB2B2B2"/>
-      </right>
-      <top style="thin">
-        <color rgb="FFB2B2B2"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FFB2B2B2"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
       <left/>
       <right/>
-      <top style="thin">
-        <color theme="4"/>
-      </top>
-      <bottom style="double">
+      <top/>
+      <bottom style="medium">
         <color theme="4"/>
       </bottom>
       <diagonal/>
@@ -988,11 +962,17 @@
       <diagonal/>
     </border>
     <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="medium">
-        <color theme="4" tint="0.499984740745262"/>
+      <left style="thin">
+        <color rgb="FFB2B2B2"/>
+      </left>
+      <right style="thin">
+        <color rgb="FFB2B2B2"/>
+      </right>
+      <top style="thin">
+        <color rgb="FFB2B2B2"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FFB2B2B2"/>
       </bottom>
       <diagonal/>
     </border>
@@ -1014,6 +994,26 @@
     <border>
       <left/>
       <right/>
+      <top style="thin">
+        <color theme="4"/>
+      </top>
+      <bottom style="double">
+        <color theme="4"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color theme="4" tint="0.499984740745262"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
       <top/>
       <bottom style="double">
         <color rgb="FFFF8001"/>
@@ -1023,148 +1023,148 @@
   </borders>
   <cellStyleXfs count="49">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="20" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="36" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="38" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="15" fillId="36" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="17" fillId="37" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="17" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="35" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="34" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="15" fillId="40" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="39" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="34" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="35" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="38" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="31" fillId="0" borderId="26" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="17" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="33" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="17" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="20" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="40" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="15" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="17" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="20" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="26" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="25" fillId="0" borderId="22" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="30" fillId="14" borderId="25" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="15" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="28" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="26" fillId="0" borderId="24" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="25" fillId="12" borderId="23" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="179" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="18" borderId="22" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="23" fillId="17" borderId="19" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="27" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="12" borderId="19" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="27" fillId="0" borderId="25" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="20" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="177" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="178" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="17" fillId="39" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="16" borderId="21" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="24" fillId="15" borderId="20" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="23" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="22" fillId="14" borderId="20" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="23" fillId="0" borderId="24" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="28" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="19" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="32" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="24" fillId="0" borderId="20" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="176" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="17" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="177" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="32" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="19" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="179" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="27" fillId="27" borderId="23" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="33" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="21" fillId="15" borderId="21" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="9" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="30" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
@@ -1226,38 +1226,38 @@
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="1" fontId="11" fillId="6" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" shrinkToFit="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="6" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="5" fillId="6" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="12" fillId="8" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="11" fillId="8" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="12" fillId="9" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="11" fillId="9" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="12" fillId="9" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="11" fillId="9" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="10" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="1" fontId="13" fillId="6" borderId="15" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" shrinkToFit="1"/>
+    </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="12" fillId="9" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="11" fillId="9" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1"/>
@@ -1561,8 +1561,8 @@
   </sheetPr>
   <dimension ref="A1:H1010"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A34" workbookViewId="0">
-      <selection activeCell="G58" sqref="G58"/>
+    <sheetView tabSelected="1" topLeftCell="A28" workbookViewId="0">
+      <selection activeCell="C46" sqref="C46:E46"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.4416666666667" defaultRowHeight="15" customHeight="1" outlineLevelCol="7"/>
@@ -1589,7 +1589,7 @@
       <c r="E1" s="2"/>
       <c r="F1" s="2"/>
       <c r="G1" s="2"/>
-      <c r="H1" s="30"/>
+      <c r="H1" s="29"/>
     </row>
     <row r="2" ht="21.75" customHeight="1" spans="1:8">
       <c r="A2" s="3" t="s">
@@ -1601,7 +1601,7 @@
       <c r="E2" s="4"/>
       <c r="F2" s="4"/>
       <c r="G2" s="4"/>
-      <c r="H2" s="30"/>
+      <c r="H2" s="29"/>
     </row>
     <row r="3" ht="16.5" customHeight="1" spans="1:8">
       <c r="A3" s="5" t="s">
@@ -1613,7 +1613,7 @@
       <c r="E3" s="6"/>
       <c r="F3" s="6"/>
       <c r="G3" s="6"/>
-      <c r="H3" s="31"/>
+      <c r="H3" s="30"/>
     </row>
     <row r="4" ht="16.5" customHeight="1" spans="1:8">
       <c r="A4" s="5" t="s">
@@ -1625,7 +1625,7 @@
       <c r="E4" s="6"/>
       <c r="F4" s="6"/>
       <c r="G4" s="6"/>
-      <c r="H4" s="31"/>
+      <c r="H4" s="30"/>
     </row>
     <row r="5" ht="16.5" customHeight="1" spans="1:8">
       <c r="A5" s="5" t="s">
@@ -1637,7 +1637,7 @@
       <c r="E5" s="6"/>
       <c r="F5" s="6"/>
       <c r="G5" s="6"/>
-      <c r="H5" s="31"/>
+      <c r="H5" s="30"/>
     </row>
     <row r="6" ht="16.5" customHeight="1" spans="1:8">
       <c r="A6" s="8" t="s">
@@ -1649,7 +1649,7 @@
       <c r="E6" s="9"/>
       <c r="F6" s="9"/>
       <c r="G6" s="9"/>
-      <c r="H6" s="31"/>
+      <c r="H6" s="30"/>
     </row>
     <row r="7" ht="16.5" customHeight="1" spans="1:8">
       <c r="A7" s="5" t="s">
@@ -1661,7 +1661,7 @@
       <c r="E7" s="10"/>
       <c r="F7" s="10"/>
       <c r="G7" s="10"/>
-      <c r="H7" s="31"/>
+      <c r="H7" s="30"/>
     </row>
     <row r="8" ht="16.5" customHeight="1" spans="1:8">
       <c r="A8" s="5" t="s">
@@ -1673,7 +1673,7 @@
       <c r="E8" s="6"/>
       <c r="F8" s="6"/>
       <c r="G8" s="6"/>
-      <c r="H8" s="31"/>
+      <c r="H8" s="30"/>
     </row>
     <row r="9" ht="12.75" customHeight="1" spans="1:7">
       <c r="A9" s="5" t="s">
@@ -1740,10 +1740,10 @@
       <c r="C14" s="16"/>
       <c r="D14" s="16"/>
       <c r="E14" s="15"/>
-      <c r="F14" s="32" t="s">
+      <c r="F14" s="31" t="s">
         <v>18</v>
       </c>
-      <c r="G14" s="33"/>
+      <c r="G14" s="32"/>
     </row>
     <row r="15" ht="19.5" customHeight="1" spans="1:7">
       <c r="A15" s="15">
@@ -1753,10 +1753,10 @@
       <c r="C15" s="16"/>
       <c r="D15" s="16"/>
       <c r="E15" s="15"/>
-      <c r="F15" s="32" t="s">
+      <c r="F15" s="31" t="s">
         <v>18</v>
       </c>
-      <c r="G15" s="33"/>
+      <c r="G15" s="32"/>
     </row>
     <row r="16" ht="19.5" customHeight="1" spans="1:7">
       <c r="A16" s="15">
@@ -1766,10 +1766,10 @@
       <c r="C16" s="17"/>
       <c r="D16" s="17"/>
       <c r="E16" s="15"/>
-      <c r="F16" s="32" t="s">
+      <c r="F16" s="31" t="s">
         <v>18</v>
       </c>
-      <c r="G16" s="33"/>
+      <c r="G16" s="32"/>
     </row>
     <row r="17" ht="19.5" customHeight="1" spans="1:7">
       <c r="A17" s="15">
@@ -1779,10 +1779,10 @@
       <c r="C17" s="17"/>
       <c r="D17" s="17"/>
       <c r="E17" s="15"/>
-      <c r="F17" s="32" t="s">
+      <c r="F17" s="31" t="s">
         <v>18</v>
       </c>
-      <c r="G17" s="33"/>
+      <c r="G17" s="32"/>
     </row>
     <row r="18" ht="19.5" customHeight="1" spans="1:7">
       <c r="A18" s="15">
@@ -1792,10 +1792,10 @@
       <c r="C18" s="17"/>
       <c r="D18" s="17"/>
       <c r="E18" s="15"/>
-      <c r="F18" s="32" t="s">
+      <c r="F18" s="31" t="s">
         <v>18</v>
       </c>
-      <c r="G18" s="33"/>
+      <c r="G18" s="32"/>
     </row>
     <row r="19" ht="19.5" customHeight="1" spans="1:7">
       <c r="A19" s="15">
@@ -1805,10 +1805,10 @@
       <c r="C19" s="17"/>
       <c r="D19" s="17"/>
       <c r="E19" s="15"/>
-      <c r="F19" s="32" t="s">
+      <c r="F19" s="31" t="s">
         <v>18</v>
       </c>
-      <c r="G19" s="33"/>
+      <c r="G19" s="32"/>
     </row>
     <row r="20" ht="19.5" customHeight="1" spans="1:7">
       <c r="A20" s="15">
@@ -1818,10 +1818,10 @@
       <c r="C20" s="17"/>
       <c r="D20" s="17"/>
       <c r="E20" s="15"/>
-      <c r="F20" s="32" t="s">
+      <c r="F20" s="31" t="s">
         <v>18</v>
       </c>
-      <c r="G20" s="33"/>
+      <c r="G20" s="32"/>
     </row>
     <row r="21" ht="19.5" customHeight="1" spans="1:7">
       <c r="A21" s="15">
@@ -1831,10 +1831,10 @@
       <c r="C21" s="17"/>
       <c r="D21" s="17"/>
       <c r="E21" s="15"/>
-      <c r="F21" s="32" t="s">
+      <c r="F21" s="31" t="s">
         <v>18</v>
       </c>
-      <c r="G21" s="33"/>
+      <c r="G21" s="32"/>
     </row>
     <row r="22" ht="19.5" customHeight="1" spans="1:7">
       <c r="A22" s="15">
@@ -1844,10 +1844,10 @@
       <c r="C22" s="17"/>
       <c r="D22" s="17"/>
       <c r="E22" s="15"/>
-      <c r="F22" s="32" t="s">
+      <c r="F22" s="31" t="s">
         <v>18</v>
       </c>
-      <c r="G22" s="33"/>
+      <c r="G22" s="32"/>
     </row>
     <row r="23" ht="19.5" customHeight="1" spans="1:7">
       <c r="A23" s="15">
@@ -1857,10 +1857,10 @@
       <c r="C23" s="17"/>
       <c r="D23" s="17"/>
       <c r="E23" s="15"/>
-      <c r="F23" s="32" t="s">
+      <c r="F23" s="31" t="s">
         <v>18</v>
       </c>
-      <c r="G23" s="33"/>
+      <c r="G23" s="32"/>
     </row>
     <row r="24" ht="19.5" customHeight="1" spans="1:7">
       <c r="A24" s="15">
@@ -1870,10 +1870,10 @@
       <c r="C24" s="17"/>
       <c r="D24" s="17"/>
       <c r="E24" s="15"/>
-      <c r="F24" s="32" t="s">
+      <c r="F24" s="31" t="s">
         <v>18</v>
       </c>
-      <c r="G24" s="33"/>
+      <c r="G24" s="32"/>
     </row>
     <row r="25" ht="19.5" customHeight="1" spans="1:7">
       <c r="A25" s="15">
@@ -1883,10 +1883,10 @@
       <c r="C25" s="17"/>
       <c r="D25" s="17"/>
       <c r="E25" s="15"/>
-      <c r="F25" s="32" t="s">
+      <c r="F25" s="31" t="s">
         <v>18</v>
       </c>
-      <c r="G25" s="33"/>
+      <c r="G25" s="32"/>
     </row>
     <row r="26" ht="19.5" customHeight="1" spans="1:7">
       <c r="A26" s="15">
@@ -1896,10 +1896,10 @@
       <c r="C26" s="17"/>
       <c r="D26" s="17"/>
       <c r="E26" s="15"/>
-      <c r="F26" s="32" t="s">
+      <c r="F26" s="31" t="s">
         <v>18</v>
       </c>
-      <c r="G26" s="33"/>
+      <c r="G26" s="32"/>
     </row>
     <row r="27" ht="19.5" customHeight="1" spans="1:7">
       <c r="A27" s="15">
@@ -1909,10 +1909,10 @@
       <c r="C27" s="17"/>
       <c r="D27" s="17"/>
       <c r="E27" s="15"/>
-      <c r="F27" s="32" t="s">
+      <c r="F27" s="31" t="s">
         <v>18</v>
       </c>
-      <c r="G27" s="33"/>
+      <c r="G27" s="32"/>
     </row>
     <row r="28" ht="19.5" customHeight="1" spans="1:7">
       <c r="A28" s="15">
@@ -1922,10 +1922,10 @@
       <c r="C28" s="17"/>
       <c r="D28" s="17"/>
       <c r="E28" s="15"/>
-      <c r="F28" s="32" t="s">
+      <c r="F28" s="31" t="s">
         <v>18</v>
       </c>
-      <c r="G28" s="33"/>
+      <c r="G28" s="32"/>
     </row>
     <row r="29" ht="19.5" customHeight="1" spans="1:7">
       <c r="A29" s="15">
@@ -1935,10 +1935,10 @@
       <c r="C29" s="17"/>
       <c r="D29" s="17"/>
       <c r="E29" s="15"/>
-      <c r="F29" s="32" t="s">
+      <c r="F29" s="31" t="s">
         <v>18</v>
       </c>
-      <c r="G29" s="33"/>
+      <c r="G29" s="32"/>
     </row>
     <row r="30" ht="19.5" customHeight="1" spans="1:7">
       <c r="A30" s="15">
@@ -1948,10 +1948,10 @@
       <c r="C30" s="17"/>
       <c r="D30" s="17"/>
       <c r="E30" s="15"/>
-      <c r="F30" s="32" t="s">
+      <c r="F30" s="31" t="s">
         <v>18</v>
       </c>
-      <c r="G30" s="33"/>
+      <c r="G30" s="32"/>
     </row>
     <row r="31" ht="19.5" customHeight="1" spans="1:7">
       <c r="A31" s="15">
@@ -1961,10 +1961,10 @@
       <c r="C31" s="17"/>
       <c r="D31" s="17"/>
       <c r="E31" s="15"/>
-      <c r="F31" s="32" t="s">
+      <c r="F31" s="31" t="s">
         <v>18</v>
       </c>
-      <c r="G31" s="33"/>
+      <c r="G31" s="32"/>
     </row>
     <row r="32" ht="19.5" customHeight="1" spans="1:7">
       <c r="A32" s="15">
@@ -1974,10 +1974,10 @@
       <c r="C32" s="17"/>
       <c r="D32" s="17"/>
       <c r="E32" s="15"/>
-      <c r="F32" s="32" t="s">
+      <c r="F32" s="31" t="s">
         <v>18</v>
       </c>
-      <c r="G32" s="33"/>
+      <c r="G32" s="32"/>
     </row>
     <row r="33" ht="19.5" customHeight="1" spans="1:7">
       <c r="A33" s="15">
@@ -1987,10 +1987,10 @@
       <c r="C33" s="17"/>
       <c r="D33" s="17"/>
       <c r="E33" s="15"/>
-      <c r="F33" s="32" t="s">
+      <c r="F33" s="31" t="s">
         <v>18</v>
       </c>
-      <c r="G33" s="33"/>
+      <c r="G33" s="32"/>
     </row>
     <row r="34" ht="19.5" customHeight="1" spans="1:7">
       <c r="A34" s="15">
@@ -2000,10 +2000,10 @@
       <c r="C34" s="17"/>
       <c r="D34" s="17"/>
       <c r="E34" s="15"/>
-      <c r="F34" s="32" t="s">
+      <c r="F34" s="31" t="s">
         <v>18</v>
       </c>
-      <c r="G34" s="33"/>
+      <c r="G34" s="32"/>
     </row>
     <row r="35" ht="19.5" customHeight="1" spans="1:7">
       <c r="A35" s="15">
@@ -2013,10 +2013,10 @@
       <c r="C35" s="17"/>
       <c r="D35" s="17"/>
       <c r="E35" s="15"/>
-      <c r="F35" s="32" t="s">
+      <c r="F35" s="31" t="s">
         <v>18</v>
       </c>
-      <c r="G35" s="33"/>
+      <c r="G35" s="32"/>
     </row>
     <row r="36" ht="19.5" customHeight="1" spans="1:7">
       <c r="A36" s="15">
@@ -2026,10 +2026,10 @@
       <c r="C36" s="17"/>
       <c r="D36" s="17"/>
       <c r="E36" s="15"/>
-      <c r="F36" s="32" t="s">
+      <c r="F36" s="31" t="s">
         <v>18</v>
       </c>
-      <c r="G36" s="33"/>
+      <c r="G36" s="32"/>
     </row>
     <row r="37" ht="19.5" customHeight="1" spans="1:7">
       <c r="A37" s="15">
@@ -2039,10 +2039,10 @@
       <c r="C37" s="17"/>
       <c r="D37" s="17"/>
       <c r="E37" s="15"/>
-      <c r="F37" s="32" t="s">
+      <c r="F37" s="31" t="s">
         <v>18</v>
       </c>
-      <c r="G37" s="33"/>
+      <c r="G37" s="32"/>
     </row>
     <row r="38" ht="19.5" customHeight="1" spans="1:7">
       <c r="A38" s="15">
@@ -2052,10 +2052,10 @@
       <c r="C38" s="17"/>
       <c r="D38" s="17"/>
       <c r="E38" s="15"/>
-      <c r="F38" s="32" t="s">
+      <c r="F38" s="31" t="s">
         <v>18</v>
       </c>
-      <c r="G38" s="33"/>
+      <c r="G38" s="32"/>
     </row>
     <row r="39" ht="19.5" customHeight="1" spans="1:7">
       <c r="A39" s="15">
@@ -2065,10 +2065,10 @@
       <c r="C39" s="17"/>
       <c r="D39" s="17"/>
       <c r="E39" s="15"/>
-      <c r="F39" s="32" t="s">
+      <c r="F39" s="31" t="s">
         <v>18</v>
       </c>
-      <c r="G39" s="33"/>
+      <c r="G39" s="32"/>
     </row>
     <row r="40" ht="19.5" customHeight="1" spans="1:7">
       <c r="A40" s="15">
@@ -2078,10 +2078,10 @@
       <c r="C40" s="17"/>
       <c r="D40" s="17"/>
       <c r="E40" s="15"/>
-      <c r="F40" s="32" t="s">
+      <c r="F40" s="31" t="s">
         <v>18</v>
       </c>
-      <c r="G40" s="33"/>
+      <c r="G40" s="32"/>
     </row>
     <row r="41" ht="19.5" customHeight="1" spans="1:7">
       <c r="A41" s="15">
@@ -2091,10 +2091,10 @@
       <c r="C41" s="17"/>
       <c r="D41" s="17"/>
       <c r="E41" s="15"/>
-      <c r="F41" s="32" t="s">
+      <c r="F41" s="31" t="s">
         <v>18</v>
       </c>
-      <c r="G41" s="33"/>
+      <c r="G41" s="32"/>
     </row>
     <row r="42" ht="19.5" customHeight="1" spans="1:7">
       <c r="A42" s="15">
@@ -2104,10 +2104,10 @@
       <c r="C42" s="17"/>
       <c r="D42" s="17"/>
       <c r="E42" s="15"/>
-      <c r="F42" s="32" t="s">
+      <c r="F42" s="31" t="s">
         <v>18</v>
       </c>
-      <c r="G42" s="33"/>
+      <c r="G42" s="32"/>
     </row>
     <row r="43" ht="19.5" customHeight="1" spans="1:7">
       <c r="A43" s="15">
@@ -2117,10 +2117,10 @@
       <c r="C43" s="17"/>
       <c r="D43" s="17"/>
       <c r="E43" s="15"/>
-      <c r="F43" s="32" t="s">
+      <c r="F43" s="31" t="s">
         <v>18</v>
       </c>
-      <c r="G43" s="33"/>
+      <c r="G43" s="32"/>
     </row>
     <row r="44" ht="19.5" customHeight="1" spans="1:7">
       <c r="A44" s="15">
@@ -2130,22 +2130,22 @@
       <c r="C44" s="17"/>
       <c r="D44" s="17"/>
       <c r="E44" s="15"/>
-      <c r="F44" s="32" t="s">
+      <c r="F44" s="31" t="s">
         <v>18</v>
       </c>
-      <c r="G44" s="33"/>
+      <c r="G44" s="32"/>
     </row>
     <row r="45" ht="19.5" customHeight="1" spans="1:3">
       <c r="A45" s="18"/>
       <c r="B45" s="18"/>
       <c r="C45" s="18"/>
     </row>
-    <row r="46" ht="19.5" customHeight="1" spans="1:3">
-      <c r="A46" s="19" t="s">
+    <row r="46" ht="19.5" customHeight="1" spans="3:5">
+      <c r="C46" s="19" t="s">
         <v>19</v>
       </c>
-      <c r="B46" s="20"/>
-      <c r="C46" s="21">
+      <c r="D46" s="20"/>
+      <c r="E46" s="33">
         <f>SUM(C14:C45)</f>
         <v>0</v>
       </c>
@@ -2153,46 +2153,46 @@
     <row r="47" ht="19.5" customHeight="1"/>
     <row r="48" ht="57.75" customHeight="1"/>
     <row r="49" ht="12.75" customHeight="1" spans="3:5">
-      <c r="C49" s="22" t="s">
+      <c r="C49" s="21" t="s">
         <v>20</v>
       </c>
-      <c r="D49" s="23"/>
+      <c r="D49" s="22"/>
       <c r="E49" s="34"/>
     </row>
     <row r="50" ht="12.75" customHeight="1" spans="3:5">
-      <c r="C50" s="24"/>
-      <c r="D50" s="23"/>
+      <c r="C50" s="23"/>
+      <c r="D50" s="22"/>
       <c r="E50" s="34"/>
     </row>
     <row r="51" ht="12.75" customHeight="1"/>
     <row r="52" ht="12.75" customHeight="1"/>
     <row r="53" ht="12.75" customHeight="1" spans="3:6">
-      <c r="C53" s="25" t="s">
+      <c r="C53" s="24" t="s">
         <v>21</v>
       </c>
-      <c r="D53" s="26"/>
-      <c r="E53" s="26"/>
+      <c r="D53" s="25"/>
+      <c r="E53" s="25"/>
       <c r="F53" s="35"/>
     </row>
     <row r="54" ht="12.75" customHeight="1" spans="3:6">
-      <c r="C54" s="27"/>
-      <c r="D54" s="28"/>
-      <c r="E54" s="28"/>
+      <c r="C54" s="26"/>
+      <c r="D54" s="27"/>
+      <c r="E54" s="27"/>
       <c r="F54" s="36"/>
     </row>
     <row r="55" ht="12.75" customHeight="1"/>
     <row r="56" ht="12.75" customHeight="1" spans="3:6">
-      <c r="C56" s="25" t="s">
+      <c r="C56" s="24" t="s">
         <v>22</v>
       </c>
-      <c r="D56" s="26"/>
-      <c r="E56" s="26"/>
+      <c r="D56" s="25"/>
+      <c r="E56" s="25"/>
       <c r="F56" s="35"/>
     </row>
     <row r="57" ht="12.75" customHeight="1" spans="3:6">
-      <c r="C57" s="27"/>
-      <c r="D57" s="29"/>
-      <c r="E57" s="29"/>
+      <c r="C57" s="26"/>
+      <c r="D57" s="28"/>
+      <c r="E57" s="28"/>
       <c r="F57" s="37"/>
     </row>
     <row r="58" ht="12.75" customHeight="1"/>
@@ -3170,7 +3170,7 @@
     <mergeCell ref="C10:G10"/>
     <mergeCell ref="A11:B11"/>
     <mergeCell ref="C11:G11"/>
-    <mergeCell ref="A46:B46"/>
+    <mergeCell ref="C46:D46"/>
     <mergeCell ref="C49:E49"/>
     <mergeCell ref="C50:E50"/>
     <mergeCell ref="C53:F53"/>

</xml_diff>

<commit_message>
refactor: adjust cell references in ExcelService and related tests
</commit_message>
<xml_diff>
--- a/src/data/model.xlsx
+++ b/src/data/model.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="3" lowestEdited="5" rupBuild="9302"/>
   <workbookPr/>
   <bookViews>
-    <workbookView windowWidth="27930" windowHeight="12495"/>
+    <workbookView windowWidth="21945" windowHeight="12495"/>
   </bookViews>
   <sheets>
     <sheet name="FREQUÊNCIA" sheetId="1" r:id="rId1"/>
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="53" uniqueCount="23">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="52" uniqueCount="22">
   <si>
     <t>JP CORPO E MENTE LTDA
 CNPJ: 49.317.168/0001-14
@@ -65,17 +65,6 @@
         <rFont val="Tahoma"/>
         <charset val="134"/>
       </rPr>
-      <t>Sessão Autorizada:</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <rPr>
-        <sz val="9"/>
-        <color theme="1"/>
-        <rFont val="Tahoma"/>
-        <charset val="134"/>
-      </rPr>
       <t>Nome paciente:</t>
     </r>
   </si>
@@ -102,10 +91,10 @@
     </r>
   </si>
   <si>
-    <t xml:space="preserve">Nº carterinha </t>
+    <t>Nº carterinha:</t>
   </si>
   <si>
-    <t>Guia Nº</t>
+    <t>Guia Nº:</t>
   </si>
   <si>
     <r>
@@ -212,10 +201,10 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="4">
-    <numFmt numFmtId="176" formatCode="_-* #,##0.00_-;\-* #,##0.00_-;_-* &quot;-&quot;??_-;_-@_-"/>
-    <numFmt numFmtId="177" formatCode="_-* #,##0_-;\-* #,##0_-;_-* &quot;-&quot;_-;_-@_-"/>
-    <numFmt numFmtId="178" formatCode="_-&quot;R$&quot;\ * #,##0_-;\-&quot;R$&quot;\ * #,##0_-;_-&quot;R$&quot;\ * &quot;-&quot;_-;_-@_-"/>
-    <numFmt numFmtId="179" formatCode="_-&quot;R$&quot;\ * #,##0.00_-;\-&quot;R$&quot;\ * #,##0.00_-;_-&quot;R$&quot;\ * &quot;-&quot;??_-;_-@_-"/>
+    <numFmt numFmtId="176" formatCode="_-&quot;R$&quot;\ * #,##0.00_-;\-&quot;R$&quot;\ * #,##0.00_-;_-&quot;R$&quot;\ * &quot;-&quot;??_-;_-@_-"/>
+    <numFmt numFmtId="177" formatCode="_-&quot;R$&quot;\ * #,##0_-;\-&quot;R$&quot;\ * #,##0_-;_-&quot;R$&quot;\ * &quot;-&quot;_-;_-@_-"/>
+    <numFmt numFmtId="178" formatCode="_-* #,##0_-;\-* #,##0_-;_-* &quot;-&quot;_-;_-@_-"/>
+    <numFmt numFmtId="179" formatCode="_-* #,##0.00_-;\-* #,##0.00_-;_-* &quot;-&quot;??_-;_-@_-"/>
   </numFmts>
   <fonts count="33">
     <font>
@@ -306,6 +295,22 @@
       <color rgb="FF000000"/>
       <name val="Tahoma"/>
       <charset val="134"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color rgb="FF0000FF"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FFFFFFFF"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
     </font>
     <font>
       <u/>
@@ -316,8 +321,38 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <b/>
+      <sz val="18"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
       <sz val="11"/>
       <color theme="0"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <i/>
+      <sz val="11"/>
+      <color rgb="FF7F7F7F"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF006100"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -331,15 +366,8 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <b/>
       <sz val="11"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="18"/>
       <color theme="3"/>
       <name val="Calibri"/>
       <charset val="134"/>
@@ -354,31 +382,30 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <i/>
+      <b/>
       <sz val="11"/>
-      <color rgb="FF7F7F7F"/>
+      <color theme="1"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
-      <b/>
       <sz val="11"/>
-      <color rgb="FFFFFFFF"/>
+      <color rgb="FF9C0006"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
       <sz val="11"/>
-      <color rgb="FF006100"/>
+      <color rgb="FFFA7D00"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
       <sz val="11"/>
-      <color rgb="FF3F3F76"/>
+      <color rgb="FF9C6500"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -392,6 +419,20 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <sz val="11"/>
+      <color rgb="FFFF0000"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF3F3F76"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
       <b/>
       <sz val="11"/>
       <color rgb="FF3F3F3F"/>
@@ -399,60 +440,8 @@
       <charset val="0"/>
       <scheme val="minor"/>
     </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF9C0006"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF9C6500"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <u/>
-      <sz val="11"/>
-      <color rgb="FF0000FF"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FFFA7D00"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FFFF0000"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
   </fonts>
-  <fills count="41">
+  <fills count="40">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -473,12 +462,6 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFBCD6ED"/>
-        <bgColor rgb="FFBCD6ED"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
         <fgColor rgb="FFF1F1F1"/>
         <bgColor indexed="64"/>
       </patternFill>
@@ -509,43 +492,157 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor rgb="FFA5A5A5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFC6EFCE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFF2F2F2"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFFCC"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFC7CE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFEB9C"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor theme="6" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="4"/>
+        <fgColor theme="7" tint="0.599993896298105"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFF2F2F2"/>
+        <fgColor theme="6" tint="0.599993896298105"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFA5A5A5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFC6EFCE"/>
+        <fgColor theme="8" tint="0.599993896298105"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -557,139 +654,25 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFFFFFCC"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFC7CE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFEB9C"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
         <fgColor theme="9"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
         <fgColor theme="5"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.399975585192419"/>
+        <fgColor theme="8" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="7" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -923,6 +906,21 @@
       <diagonal/>
     </border>
     <border>
+      <left style="double">
+        <color rgb="FF3F3F3F"/>
+      </left>
+      <right style="double">
+        <color rgb="FF3F3F3F"/>
+      </right>
+      <top style="double">
+        <color rgb="FF3F3F3F"/>
+      </top>
+      <bottom style="double">
+        <color rgb="FF3F3F3F"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
       <left style="thin">
         <color rgb="FF7F7F7F"/>
       </left>
@@ -947,21 +945,6 @@
       <diagonal/>
     </border>
     <border>
-      <left style="double">
-        <color rgb="FF3F3F3F"/>
-      </left>
-      <right style="double">
-        <color rgb="FF3F3F3F"/>
-      </right>
-      <top style="double">
-        <color rgb="FF3F3F3F"/>
-      </top>
-      <bottom style="double">
-        <color rgb="FF3F3F3F"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
       <left style="thin">
         <color rgb="FFB2B2B2"/>
       </left>
@@ -973,6 +956,26 @@
       </top>
       <bottom style="thin">
         <color rgb="FFB2B2B2"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color theme="4"/>
+      </top>
+      <bottom style="double">
+        <color theme="4"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="double">
+        <color rgb="FFFF8001"/>
       </bottom>
       <diagonal/>
     </border>
@@ -994,181 +997,161 @@
     <border>
       <left/>
       <right/>
-      <top style="thin">
-        <color theme="4"/>
-      </top>
-      <bottom style="double">
-        <color theme="4"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
       <top/>
       <bottom style="medium">
         <color theme="4" tint="0.499984740745262"/>
       </bottom>
       <diagonal/>
     </border>
-    <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="double">
-        <color rgb="FFFF8001"/>
-      </bottom>
-      <diagonal/>
-    </border>
   </borders>
   <cellStyleXfs count="49">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="15" fillId="36" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="37" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="40" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="39" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="34" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="35" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="38" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="31" fillId="0" borderId="26" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="33" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="29" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="28" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="26" fillId="0" borderId="24" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="25" fillId="12" borderId="23" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="19" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="38" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="36" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="34" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="39" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="27" fillId="0" borderId="24" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="33" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="37" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="28" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="26" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="25" fillId="0" borderId="23" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="32" fillId="14" borderId="25" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="176" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="15" borderId="22" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="31" fillId="35" borderId="20" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="23" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="14" borderId="20" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="23" fillId="0" borderId="26" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="24" fillId="0" borderId="21" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="178" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="177" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="30" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="21" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="179" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="17" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="18" borderId="22" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="23" fillId="17" borderId="19" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="27" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="12" borderId="19" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="22" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="27" fillId="0" borderId="25" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="0" borderId="20" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="177" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="178" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="32" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="15" fillId="9" borderId="19" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="24" fillId="0" borderId="20" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="176" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="15" borderId="21" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="30" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
   </cellStyleXfs>
-  <cellXfs count="38">
+  <cellXfs count="36">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
@@ -1189,31 +1172,25 @@
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="3" fillId="4" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="4" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="5" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="5" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="6" fillId="4" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="5" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="6" fillId="4" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="5" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="6" fillId="4" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="6" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="7" fillId="5" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="1" fontId="8" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" shrinkToFit="1"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="7" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="9" fillId="6" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" shrinkToFit="1"/>
     </xf>
     <xf numFmtId="0" fontId="9" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -1222,25 +1199,25 @@
     <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="6" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="7" fillId="5" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="5" fillId="6" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="5" fillId="5" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="10" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="8" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="11" fillId="7" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="11" fillId="9" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="11" fillId="8" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="9" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="11" fillId="8" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1"/>
@@ -1252,12 +1229,12 @@
     <xf numFmtId="0" fontId="10" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="1" fontId="13" fillId="6" borderId="15" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="1" fontId="13" fillId="5" borderId="15" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" shrinkToFit="1"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="11" fillId="9" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="11" fillId="8" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1"/>
@@ -1561,8 +1538,8 @@
   </sheetPr>
   <dimension ref="A1:H1010"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A28" workbookViewId="0">
-      <selection activeCell="C46" sqref="C46:E46"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A10" sqref="A10:B10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.4416666666667" defaultRowHeight="15" customHeight="1" outlineLevelCol="7"/>
@@ -1589,7 +1566,7 @@
       <c r="E1" s="2"/>
       <c r="F1" s="2"/>
       <c r="G1" s="2"/>
-      <c r="H1" s="29"/>
+      <c r="H1" s="27"/>
     </row>
     <row r="2" ht="21.75" customHeight="1" spans="1:8">
       <c r="A2" s="3" t="s">
@@ -1601,7 +1578,7 @@
       <c r="E2" s="4"/>
       <c r="F2" s="4"/>
       <c r="G2" s="4"/>
-      <c r="H2" s="29"/>
+      <c r="H2" s="27"/>
     </row>
     <row r="3" ht="16.5" customHeight="1" spans="1:8">
       <c r="A3" s="5" t="s">
@@ -1613,7 +1590,7 @@
       <c r="E3" s="6"/>
       <c r="F3" s="6"/>
       <c r="G3" s="6"/>
-      <c r="H3" s="30"/>
+      <c r="H3" s="28"/>
     </row>
     <row r="4" ht="16.5" customHeight="1" spans="1:8">
       <c r="A4" s="5" t="s">
@@ -1625,7 +1602,7 @@
       <c r="E4" s="6"/>
       <c r="F4" s="6"/>
       <c r="G4" s="6"/>
-      <c r="H4" s="30"/>
+      <c r="H4" s="28"/>
     </row>
     <row r="5" ht="16.5" customHeight="1" spans="1:8">
       <c r="A5" s="5" t="s">
@@ -1637,31 +1614,31 @@
       <c r="E5" s="6"/>
       <c r="F5" s="6"/>
       <c r="G5" s="6"/>
-      <c r="H5" s="30"/>
+      <c r="H5" s="28"/>
     </row>
     <row r="6" ht="16.5" customHeight="1" spans="1:8">
-      <c r="A6" s="8" t="s">
+      <c r="A6" s="5" t="s">
         <v>5</v>
       </c>
       <c r="B6" s="7"/>
-      <c r="C6" s="9"/>
-      <c r="D6" s="9"/>
-      <c r="E6" s="9"/>
-      <c r="F6" s="9"/>
-      <c r="G6" s="9"/>
-      <c r="H6" s="30"/>
+      <c r="C6" s="8"/>
+      <c r="D6" s="8"/>
+      <c r="E6" s="8"/>
+      <c r="F6" s="8"/>
+      <c r="G6" s="8"/>
+      <c r="H6" s="28"/>
     </row>
     <row r="7" ht="16.5" customHeight="1" spans="1:8">
       <c r="A7" s="5" t="s">
         <v>6</v>
       </c>
       <c r="B7" s="7"/>
-      <c r="C7" s="10"/>
-      <c r="D7" s="10"/>
-      <c r="E7" s="10"/>
-      <c r="F7" s="10"/>
-      <c r="G7" s="10"/>
-      <c r="H7" s="30"/>
+      <c r="C7" s="6"/>
+      <c r="D7" s="6"/>
+      <c r="E7" s="6"/>
+      <c r="F7" s="6"/>
+      <c r="G7" s="6"/>
+      <c r="H7" s="28"/>
     </row>
     <row r="8" ht="16.5" customHeight="1" spans="1:8">
       <c r="A8" s="5" t="s">
@@ -1673,13 +1650,13 @@
       <c r="E8" s="6"/>
       <c r="F8" s="6"/>
       <c r="G8" s="6"/>
-      <c r="H8" s="30"/>
+      <c r="H8" s="28"/>
     </row>
     <row r="9" ht="12.75" customHeight="1" spans="1:7">
-      <c r="A9" s="5" t="s">
+      <c r="A9" s="9" t="s">
         <v>8</v>
       </c>
-      <c r="B9" s="7"/>
+      <c r="B9" s="10"/>
       <c r="C9" s="6"/>
       <c r="D9" s="6"/>
       <c r="E9" s="6"/>
@@ -1690,511 +1667,501 @@
       <c r="A10" s="11" t="s">
         <v>9</v>
       </c>
-      <c r="B10" s="12"/>
+      <c r="B10" s="11"/>
       <c r="C10" s="6"/>
       <c r="D10" s="6"/>
       <c r="E10" s="6"/>
       <c r="F10" s="6"/>
       <c r="G10" s="6"/>
     </row>
-    <row r="11" ht="19.5" customHeight="1" spans="1:7">
-      <c r="A11" s="13" t="s">
+    <row r="11" ht="19.5" customHeight="1"/>
+    <row r="12" ht="19.5" customHeight="1" spans="1:7">
+      <c r="A12" s="12" t="s">
         <v>10</v>
       </c>
-      <c r="B11" s="13"/>
-      <c r="C11" s="6"/>
-      <c r="D11" s="6"/>
-      <c r="E11" s="6"/>
-      <c r="F11" s="6"/>
-      <c r="G11" s="6"/>
-    </row>
-    <row r="12" ht="19.5" customHeight="1"/>
+      <c r="B12" s="12" t="s">
+        <v>11</v>
+      </c>
+      <c r="C12" s="12" t="s">
+        <v>12</v>
+      </c>
+      <c r="D12" s="12" t="s">
+        <v>13</v>
+      </c>
+      <c r="E12" s="12" t="s">
+        <v>14</v>
+      </c>
+      <c r="F12" s="12" t="s">
+        <v>15</v>
+      </c>
+      <c r="G12" s="12" t="s">
+        <v>16</v>
+      </c>
+    </row>
     <row r="13" ht="19.5" customHeight="1" spans="1:7">
-      <c r="A13" s="14" t="s">
+      <c r="A13" s="13">
+        <v>1</v>
+      </c>
+      <c r="B13" s="14"/>
+      <c r="C13" s="14"/>
+      <c r="D13" s="14"/>
+      <c r="E13" s="13"/>
+      <c r="F13" s="29" t="s">
+        <v>17</v>
+      </c>
+      <c r="G13" s="30"/>
+    </row>
+    <row r="14" ht="19.5" customHeight="1" spans="1:7">
+      <c r="A14" s="13">
+        <v>2</v>
+      </c>
+      <c r="B14" s="14"/>
+      <c r="C14" s="14"/>
+      <c r="D14" s="14"/>
+      <c r="E14" s="13"/>
+      <c r="F14" s="29" t="s">
+        <v>17</v>
+      </c>
+      <c r="G14" s="30"/>
+    </row>
+    <row r="15" ht="19.5" customHeight="1" spans="1:7">
+      <c r="A15" s="13">
+        <v>3</v>
+      </c>
+      <c r="B15" s="15"/>
+      <c r="C15" s="15"/>
+      <c r="D15" s="15"/>
+      <c r="E15" s="13"/>
+      <c r="F15" s="29" t="s">
+        <v>17</v>
+      </c>
+      <c r="G15" s="30"/>
+    </row>
+    <row r="16" ht="19.5" customHeight="1" spans="1:7">
+      <c r="A16" s="13">
+        <v>4</v>
+      </c>
+      <c r="B16" s="15"/>
+      <c r="C16" s="15"/>
+      <c r="D16" s="15"/>
+      <c r="E16" s="13"/>
+      <c r="F16" s="29" t="s">
+        <v>17</v>
+      </c>
+      <c r="G16" s="30"/>
+    </row>
+    <row r="17" ht="19.5" customHeight="1" spans="1:7">
+      <c r="A17" s="13">
+        <v>5</v>
+      </c>
+      <c r="B17" s="15"/>
+      <c r="C17" s="15"/>
+      <c r="D17" s="15"/>
+      <c r="E17" s="13"/>
+      <c r="F17" s="29" t="s">
+        <v>17</v>
+      </c>
+      <c r="G17" s="30"/>
+    </row>
+    <row r="18" ht="19.5" customHeight="1" spans="1:7">
+      <c r="A18" s="13">
+        <v>6</v>
+      </c>
+      <c r="B18" s="15"/>
+      <c r="C18" s="15"/>
+      <c r="D18" s="15"/>
+      <c r="E18" s="13"/>
+      <c r="F18" s="29" t="s">
+        <v>17</v>
+      </c>
+      <c r="G18" s="30"/>
+    </row>
+    <row r="19" ht="19.5" customHeight="1" spans="1:7">
+      <c r="A19" s="13">
+        <v>7</v>
+      </c>
+      <c r="B19" s="15"/>
+      <c r="C19" s="15"/>
+      <c r="D19" s="15"/>
+      <c r="E19" s="13"/>
+      <c r="F19" s="29" t="s">
+        <v>17</v>
+      </c>
+      <c r="G19" s="30"/>
+    </row>
+    <row r="20" ht="19.5" customHeight="1" spans="1:7">
+      <c r="A20" s="13">
+        <v>8</v>
+      </c>
+      <c r="B20" s="15"/>
+      <c r="C20" s="15"/>
+      <c r="D20" s="15"/>
+      <c r="E20" s="13"/>
+      <c r="F20" s="29" t="s">
+        <v>17</v>
+      </c>
+      <c r="G20" s="30"/>
+    </row>
+    <row r="21" ht="19.5" customHeight="1" spans="1:7">
+      <c r="A21" s="13">
+        <v>9</v>
+      </c>
+      <c r="B21" s="15"/>
+      <c r="C21" s="15"/>
+      <c r="D21" s="15"/>
+      <c r="E21" s="13"/>
+      <c r="F21" s="29" t="s">
+        <v>17</v>
+      </c>
+      <c r="G21" s="30"/>
+    </row>
+    <row r="22" ht="19.5" customHeight="1" spans="1:7">
+      <c r="A22" s="13">
+        <v>10</v>
+      </c>
+      <c r="B22" s="15"/>
+      <c r="C22" s="15"/>
+      <c r="D22" s="15"/>
+      <c r="E22" s="13"/>
+      <c r="F22" s="29" t="s">
+        <v>17</v>
+      </c>
+      <c r="G22" s="30"/>
+    </row>
+    <row r="23" ht="19.5" customHeight="1" spans="1:7">
+      <c r="A23" s="13">
         <v>11</v>
       </c>
-      <c r="B13" s="14" t="s">
+      <c r="B23" s="15"/>
+      <c r="C23" s="15"/>
+      <c r="D23" s="15"/>
+      <c r="E23" s="13"/>
+      <c r="F23" s="29" t="s">
+        <v>17</v>
+      </c>
+      <c r="G23" s="30"/>
+    </row>
+    <row r="24" ht="19.5" customHeight="1" spans="1:7">
+      <c r="A24" s="13">
         <v>12</v>
       </c>
-      <c r="C13" s="14" t="s">
+      <c r="B24" s="15"/>
+      <c r="C24" s="15"/>
+      <c r="D24" s="15"/>
+      <c r="E24" s="13"/>
+      <c r="F24" s="29" t="s">
+        <v>17</v>
+      </c>
+      <c r="G24" s="30"/>
+    </row>
+    <row r="25" ht="19.5" customHeight="1" spans="1:7">
+      <c r="A25" s="13">
         <v>13</v>
       </c>
-      <c r="D13" s="14" t="s">
+      <c r="B25" s="15"/>
+      <c r="C25" s="15"/>
+      <c r="D25" s="15"/>
+      <c r="E25" s="13"/>
+      <c r="F25" s="29" t="s">
+        <v>17</v>
+      </c>
+      <c r="G25" s="30"/>
+    </row>
+    <row r="26" ht="19.5" customHeight="1" spans="1:7">
+      <c r="A26" s="13">
         <v>14</v>
       </c>
-      <c r="E13" s="14" t="s">
+      <c r="B26" s="15"/>
+      <c r="C26" s="15"/>
+      <c r="D26" s="15"/>
+      <c r="E26" s="13"/>
+      <c r="F26" s="29" t="s">
+        <v>17</v>
+      </c>
+      <c r="G26" s="30"/>
+    </row>
+    <row r="27" ht="19.5" customHeight="1" spans="1:7">
+      <c r="A27" s="13">
         <v>15</v>
       </c>
-      <c r="F13" s="14" t="s">
+      <c r="B27" s="15"/>
+      <c r="C27" s="15"/>
+      <c r="D27" s="15"/>
+      <c r="E27" s="13"/>
+      <c r="F27" s="29" t="s">
+        <v>17</v>
+      </c>
+      <c r="G27" s="30"/>
+    </row>
+    <row r="28" ht="19.5" customHeight="1" spans="1:7">
+      <c r="A28" s="13">
         <v>16</v>
       </c>
-      <c r="G13" s="14" t="s">
+      <c r="B28" s="15"/>
+      <c r="C28" s="15"/>
+      <c r="D28" s="15"/>
+      <c r="E28" s="13"/>
+      <c r="F28" s="29" t="s">
         <v>17</v>
       </c>
-    </row>
-    <row r="14" ht="19.5" customHeight="1" spans="1:7">
-      <c r="A14" s="15">
-        <v>1</v>
-      </c>
-      <c r="B14" s="16"/>
-      <c r="C14" s="16"/>
-      <c r="D14" s="16"/>
-      <c r="E14" s="15"/>
-      <c r="F14" s="31" t="s">
+      <c r="G28" s="30"/>
+    </row>
+    <row r="29" ht="19.5" customHeight="1" spans="1:7">
+      <c r="A29" s="13">
+        <v>17</v>
+      </c>
+      <c r="B29" s="15"/>
+      <c r="C29" s="15"/>
+      <c r="D29" s="15"/>
+      <c r="E29" s="13"/>
+      <c r="F29" s="29" t="s">
+        <v>17</v>
+      </c>
+      <c r="G29" s="30"/>
+    </row>
+    <row r="30" ht="19.5" customHeight="1" spans="1:7">
+      <c r="A30" s="13">
         <v>18</v>
       </c>
-      <c r="G14" s="32"/>
-    </row>
-    <row r="15" ht="19.5" customHeight="1" spans="1:7">
-      <c r="A15" s="15">
-        <v>2</v>
-      </c>
-      <c r="B15" s="16"/>
-      <c r="C15" s="16"/>
-      <c r="D15" s="16"/>
-      <c r="E15" s="15"/>
-      <c r="F15" s="31" t="s">
+      <c r="B30" s="15"/>
+      <c r="C30" s="15"/>
+      <c r="D30" s="15"/>
+      <c r="E30" s="13"/>
+      <c r="F30" s="29" t="s">
+        <v>17</v>
+      </c>
+      <c r="G30" s="30"/>
+    </row>
+    <row r="31" ht="19.5" customHeight="1" spans="1:7">
+      <c r="A31" s="13">
+        <v>19</v>
+      </c>
+      <c r="B31" s="15"/>
+      <c r="C31" s="15"/>
+      <c r="D31" s="15"/>
+      <c r="E31" s="13"/>
+      <c r="F31" s="29" t="s">
+        <v>17</v>
+      </c>
+      <c r="G31" s="30"/>
+    </row>
+    <row r="32" ht="19.5" customHeight="1" spans="1:7">
+      <c r="A32" s="13">
+        <v>20</v>
+      </c>
+      <c r="B32" s="15"/>
+      <c r="C32" s="15"/>
+      <c r="D32" s="15"/>
+      <c r="E32" s="13"/>
+      <c r="F32" s="29" t="s">
+        <v>17</v>
+      </c>
+      <c r="G32" s="30"/>
+    </row>
+    <row r="33" ht="19.5" customHeight="1" spans="1:7">
+      <c r="A33" s="13">
+        <v>21</v>
+      </c>
+      <c r="B33" s="15"/>
+      <c r="C33" s="15"/>
+      <c r="D33" s="15"/>
+      <c r="E33" s="13"/>
+      <c r="F33" s="29" t="s">
+        <v>17</v>
+      </c>
+      <c r="G33" s="30"/>
+    </row>
+    <row r="34" ht="19.5" customHeight="1" spans="1:7">
+      <c r="A34" s="13">
+        <v>22</v>
+      </c>
+      <c r="B34" s="15"/>
+      <c r="C34" s="15"/>
+      <c r="D34" s="15"/>
+      <c r="E34" s="13"/>
+      <c r="F34" s="29" t="s">
+        <v>17</v>
+      </c>
+      <c r="G34" s="30"/>
+    </row>
+    <row r="35" ht="19.5" customHeight="1" spans="1:7">
+      <c r="A35" s="13">
+        <v>23</v>
+      </c>
+      <c r="B35" s="15"/>
+      <c r="C35" s="15"/>
+      <c r="D35" s="15"/>
+      <c r="E35" s="13"/>
+      <c r="F35" s="29" t="s">
+        <v>17</v>
+      </c>
+      <c r="G35" s="30"/>
+    </row>
+    <row r="36" ht="19.5" customHeight="1" spans="1:7">
+      <c r="A36" s="13">
+        <v>24</v>
+      </c>
+      <c r="B36" s="15"/>
+      <c r="C36" s="15"/>
+      <c r="D36" s="15"/>
+      <c r="E36" s="13"/>
+      <c r="F36" s="29" t="s">
+        <v>17</v>
+      </c>
+      <c r="G36" s="30"/>
+    </row>
+    <row r="37" ht="19.5" customHeight="1" spans="1:7">
+      <c r="A37" s="13">
+        <v>25</v>
+      </c>
+      <c r="B37" s="15"/>
+      <c r="C37" s="15"/>
+      <c r="D37" s="15"/>
+      <c r="E37" s="13"/>
+      <c r="F37" s="29" t="s">
+        <v>17</v>
+      </c>
+      <c r="G37" s="30"/>
+    </row>
+    <row r="38" ht="19.5" customHeight="1" spans="1:7">
+      <c r="A38" s="13">
+        <v>26</v>
+      </c>
+      <c r="B38" s="15"/>
+      <c r="C38" s="15"/>
+      <c r="D38" s="15"/>
+      <c r="E38" s="13"/>
+      <c r="F38" s="29" t="s">
+        <v>17</v>
+      </c>
+      <c r="G38" s="30"/>
+    </row>
+    <row r="39" ht="19.5" customHeight="1" spans="1:7">
+      <c r="A39" s="13">
+        <v>27</v>
+      </c>
+      <c r="B39" s="15"/>
+      <c r="C39" s="15"/>
+      <c r="D39" s="15"/>
+      <c r="E39" s="13"/>
+      <c r="F39" s="29" t="s">
+        <v>17</v>
+      </c>
+      <c r="G39" s="30"/>
+    </row>
+    <row r="40" ht="19.5" customHeight="1" spans="1:7">
+      <c r="A40" s="13">
+        <v>28</v>
+      </c>
+      <c r="B40" s="15"/>
+      <c r="C40" s="15"/>
+      <c r="D40" s="15"/>
+      <c r="E40" s="13"/>
+      <c r="F40" s="29" t="s">
+        <v>17</v>
+      </c>
+      <c r="G40" s="30"/>
+    </row>
+    <row r="41" ht="19.5" customHeight="1" spans="1:7">
+      <c r="A41" s="13">
+        <v>29</v>
+      </c>
+      <c r="B41" s="15"/>
+      <c r="C41" s="15"/>
+      <c r="D41" s="15"/>
+      <c r="E41" s="13"/>
+      <c r="F41" s="29" t="s">
+        <v>17</v>
+      </c>
+      <c r="G41" s="30"/>
+    </row>
+    <row r="42" ht="19.5" customHeight="1" spans="1:7">
+      <c r="A42" s="13">
+        <v>30</v>
+      </c>
+      <c r="B42" s="15"/>
+      <c r="C42" s="15"/>
+      <c r="D42" s="15"/>
+      <c r="E42" s="13"/>
+      <c r="F42" s="29" t="s">
+        <v>17</v>
+      </c>
+      <c r="G42" s="30"/>
+    </row>
+    <row r="43" ht="19.5" customHeight="1" spans="1:7">
+      <c r="A43" s="13">
+        <v>31</v>
+      </c>
+      <c r="B43" s="15"/>
+      <c r="C43" s="15"/>
+      <c r="D43" s="15"/>
+      <c r="E43" s="13"/>
+      <c r="F43" s="29" t="s">
+        <v>17</v>
+      </c>
+      <c r="G43" s="30"/>
+    </row>
+    <row r="44" ht="19.5" customHeight="1" spans="1:3">
+      <c r="A44" s="16"/>
+      <c r="B44" s="16"/>
+      <c r="C44" s="16"/>
+    </row>
+    <row r="45" ht="19.5" customHeight="1" spans="3:5">
+      <c r="C45" s="17" t="s">
         <v>18</v>
       </c>
-      <c r="G15" s="32"/>
-    </row>
-    <row r="16" ht="19.5" customHeight="1" spans="1:7">
-      <c r="A16" s="15">
-        <v>3</v>
-      </c>
-      <c r="B16" s="17"/>
-      <c r="C16" s="17"/>
-      <c r="D16" s="17"/>
-      <c r="E16" s="15"/>
-      <c r="F16" s="31" t="s">
-        <v>18</v>
-      </c>
-      <c r="G16" s="32"/>
-    </row>
-    <row r="17" ht="19.5" customHeight="1" spans="1:7">
-      <c r="A17" s="15">
-        <v>4</v>
-      </c>
-      <c r="B17" s="17"/>
-      <c r="C17" s="17"/>
-      <c r="D17" s="17"/>
-      <c r="E17" s="15"/>
-      <c r="F17" s="31" t="s">
-        <v>18</v>
-      </c>
-      <c r="G17" s="32"/>
-    </row>
-    <row r="18" ht="19.5" customHeight="1" spans="1:7">
-      <c r="A18" s="15">
-        <v>5</v>
-      </c>
-      <c r="B18" s="17"/>
-      <c r="C18" s="17"/>
-      <c r="D18" s="17"/>
-      <c r="E18" s="15"/>
-      <c r="F18" s="31" t="s">
-        <v>18</v>
-      </c>
-      <c r="G18" s="32"/>
-    </row>
-    <row r="19" ht="19.5" customHeight="1" spans="1:7">
-      <c r="A19" s="15">
-        <v>6</v>
-      </c>
-      <c r="B19" s="17"/>
-      <c r="C19" s="17"/>
-      <c r="D19" s="17"/>
-      <c r="E19" s="15"/>
-      <c r="F19" s="31" t="s">
-        <v>18</v>
-      </c>
-      <c r="G19" s="32"/>
-    </row>
-    <row r="20" ht="19.5" customHeight="1" spans="1:7">
-      <c r="A20" s="15">
-        <v>7</v>
-      </c>
-      <c r="B20" s="17"/>
-      <c r="C20" s="17"/>
-      <c r="D20" s="17"/>
-      <c r="E20" s="15"/>
-      <c r="F20" s="31" t="s">
-        <v>18</v>
-      </c>
-      <c r="G20" s="32"/>
-    </row>
-    <row r="21" ht="19.5" customHeight="1" spans="1:7">
-      <c r="A21" s="15">
-        <v>8</v>
-      </c>
-      <c r="B21" s="17"/>
-      <c r="C21" s="17"/>
-      <c r="D21" s="17"/>
-      <c r="E21" s="15"/>
-      <c r="F21" s="31" t="s">
-        <v>18</v>
-      </c>
-      <c r="G21" s="32"/>
-    </row>
-    <row r="22" ht="19.5" customHeight="1" spans="1:7">
-      <c r="A22" s="15">
-        <v>9</v>
-      </c>
-      <c r="B22" s="17"/>
-      <c r="C22" s="17"/>
-      <c r="D22" s="17"/>
-      <c r="E22" s="15"/>
-      <c r="F22" s="31" t="s">
-        <v>18</v>
-      </c>
-      <c r="G22" s="32"/>
-    </row>
-    <row r="23" ht="19.5" customHeight="1" spans="1:7">
-      <c r="A23" s="15">
-        <v>10</v>
-      </c>
-      <c r="B23" s="17"/>
-      <c r="C23" s="17"/>
-      <c r="D23" s="17"/>
-      <c r="E23" s="15"/>
-      <c r="F23" s="31" t="s">
-        <v>18</v>
-      </c>
-      <c r="G23" s="32"/>
-    </row>
-    <row r="24" ht="19.5" customHeight="1" spans="1:7">
-      <c r="A24" s="15">
-        <v>11</v>
-      </c>
-      <c r="B24" s="17"/>
-      <c r="C24" s="17"/>
-      <c r="D24" s="17"/>
-      <c r="E24" s="15"/>
-      <c r="F24" s="31" t="s">
-        <v>18</v>
-      </c>
-      <c r="G24" s="32"/>
-    </row>
-    <row r="25" ht="19.5" customHeight="1" spans="1:7">
-      <c r="A25" s="15">
-        <v>12</v>
-      </c>
-      <c r="B25" s="17"/>
-      <c r="C25" s="17"/>
-      <c r="D25" s="17"/>
-      <c r="E25" s="15"/>
-      <c r="F25" s="31" t="s">
-        <v>18</v>
-      </c>
-      <c r="G25" s="32"/>
-    </row>
-    <row r="26" ht="19.5" customHeight="1" spans="1:7">
-      <c r="A26" s="15">
-        <v>13</v>
-      </c>
-      <c r="B26" s="17"/>
-      <c r="C26" s="17"/>
-      <c r="D26" s="17"/>
-      <c r="E26" s="15"/>
-      <c r="F26" s="31" t="s">
-        <v>18</v>
-      </c>
-      <c r="G26" s="32"/>
-    </row>
-    <row r="27" ht="19.5" customHeight="1" spans="1:7">
-      <c r="A27" s="15">
-        <v>14</v>
-      </c>
-      <c r="B27" s="17"/>
-      <c r="C27" s="17"/>
-      <c r="D27" s="17"/>
-      <c r="E27" s="15"/>
-      <c r="F27" s="31" t="s">
-        <v>18</v>
-      </c>
-      <c r="G27" s="32"/>
-    </row>
-    <row r="28" ht="19.5" customHeight="1" spans="1:7">
-      <c r="A28" s="15">
-        <v>15</v>
-      </c>
-      <c r="B28" s="17"/>
-      <c r="C28" s="17"/>
-      <c r="D28" s="17"/>
-      <c r="E28" s="15"/>
-      <c r="F28" s="31" t="s">
-        <v>18</v>
-      </c>
-      <c r="G28" s="32"/>
-    </row>
-    <row r="29" ht="19.5" customHeight="1" spans="1:7">
-      <c r="A29" s="15">
-        <v>16</v>
-      </c>
-      <c r="B29" s="17"/>
-      <c r="C29" s="17"/>
-      <c r="D29" s="17"/>
-      <c r="E29" s="15"/>
-      <c r="F29" s="31" t="s">
-        <v>18</v>
-      </c>
-      <c r="G29" s="32"/>
-    </row>
-    <row r="30" ht="19.5" customHeight="1" spans="1:7">
-      <c r="A30" s="15">
-        <v>17</v>
-      </c>
-      <c r="B30" s="17"/>
-      <c r="C30" s="17"/>
-      <c r="D30" s="17"/>
-      <c r="E30" s="15"/>
-      <c r="F30" s="31" t="s">
-        <v>18</v>
-      </c>
-      <c r="G30" s="32"/>
-    </row>
-    <row r="31" ht="19.5" customHeight="1" spans="1:7">
-      <c r="A31" s="15">
-        <v>18</v>
-      </c>
-      <c r="B31" s="17"/>
-      <c r="C31" s="17"/>
-      <c r="D31" s="17"/>
-      <c r="E31" s="15"/>
-      <c r="F31" s="31" t="s">
-        <v>18</v>
-      </c>
-      <c r="G31" s="32"/>
-    </row>
-    <row r="32" ht="19.5" customHeight="1" spans="1:7">
-      <c r="A32" s="15">
+      <c r="D45" s="18"/>
+      <c r="E45" s="31">
+        <f>SUM(C13:C44)</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="46" ht="19.5" customHeight="1"/>
+    <row r="47" ht="19.5" customHeight="1"/>
+    <row r="48" ht="57.75" customHeight="1" spans="3:5">
+      <c r="C48" s="19" t="s">
         <v>19</v>
       </c>
-      <c r="B32" s="17"/>
-      <c r="C32" s="17"/>
-      <c r="D32" s="17"/>
-      <c r="E32" s="15"/>
-      <c r="F32" s="31" t="s">
-        <v>18</v>
-      </c>
-      <c r="G32" s="32"/>
-    </row>
-    <row r="33" ht="19.5" customHeight="1" spans="1:7">
-      <c r="A33" s="15">
+      <c r="D48" s="20"/>
+      <c r="E48" s="32"/>
+    </row>
+    <row r="49" ht="12.75" customHeight="1" spans="3:5">
+      <c r="C49" s="21"/>
+      <c r="D49" s="20"/>
+      <c r="E49" s="32"/>
+    </row>
+    <row r="50" ht="12.75" customHeight="1"/>
+    <row r="51" ht="12.75" customHeight="1"/>
+    <row r="52" ht="12.75" customHeight="1" spans="3:6">
+      <c r="C52" s="22" t="s">
         <v>20</v>
       </c>
-      <c r="B33" s="17"/>
-      <c r="C33" s="17"/>
-      <c r="D33" s="17"/>
-      <c r="E33" s="15"/>
-      <c r="F33" s="31" t="s">
-        <v>18</v>
-      </c>
-      <c r="G33" s="32"/>
-    </row>
-    <row r="34" ht="19.5" customHeight="1" spans="1:7">
-      <c r="A34" s="15">
-        <v>21</v>
-      </c>
-      <c r="B34" s="17"/>
-      <c r="C34" s="17"/>
-      <c r="D34" s="17"/>
-      <c r="E34" s="15"/>
-      <c r="F34" s="31" t="s">
-        <v>18</v>
-      </c>
-      <c r="G34" s="32"/>
-    </row>
-    <row r="35" ht="19.5" customHeight="1" spans="1:7">
-      <c r="A35" s="15">
-        <v>22</v>
-      </c>
-      <c r="B35" s="17"/>
-      <c r="C35" s="17"/>
-      <c r="D35" s="17"/>
-      <c r="E35" s="15"/>
-      <c r="F35" s="31" t="s">
-        <v>18</v>
-      </c>
-      <c r="G35" s="32"/>
-    </row>
-    <row r="36" ht="19.5" customHeight="1" spans="1:7">
-      <c r="A36" s="15">
-        <v>23</v>
-      </c>
-      <c r="B36" s="17"/>
-      <c r="C36" s="17"/>
-      <c r="D36" s="17"/>
-      <c r="E36" s="15"/>
-      <c r="F36" s="31" t="s">
-        <v>18</v>
-      </c>
-      <c r="G36" s="32"/>
-    </row>
-    <row r="37" ht="19.5" customHeight="1" spans="1:7">
-      <c r="A37" s="15">
-        <v>24</v>
-      </c>
-      <c r="B37" s="17"/>
-      <c r="C37" s="17"/>
-      <c r="D37" s="17"/>
-      <c r="E37" s="15"/>
-      <c r="F37" s="31" t="s">
-        <v>18</v>
-      </c>
-      <c r="G37" s="32"/>
-    </row>
-    <row r="38" ht="19.5" customHeight="1" spans="1:7">
-      <c r="A38" s="15">
-        <v>25</v>
-      </c>
-      <c r="B38" s="17"/>
-      <c r="C38" s="17"/>
-      <c r="D38" s="17"/>
-      <c r="E38" s="15"/>
-      <c r="F38" s="31" t="s">
-        <v>18</v>
-      </c>
-      <c r="G38" s="32"/>
-    </row>
-    <row r="39" ht="19.5" customHeight="1" spans="1:7">
-      <c r="A39" s="15">
-        <v>26</v>
-      </c>
-      <c r="B39" s="17"/>
-      <c r="C39" s="17"/>
-      <c r="D39" s="17"/>
-      <c r="E39" s="15"/>
-      <c r="F39" s="31" t="s">
-        <v>18</v>
-      </c>
-      <c r="G39" s="32"/>
-    </row>
-    <row r="40" ht="19.5" customHeight="1" spans="1:7">
-      <c r="A40" s="15">
-        <v>27</v>
-      </c>
-      <c r="B40" s="17"/>
-      <c r="C40" s="17"/>
-      <c r="D40" s="17"/>
-      <c r="E40" s="15"/>
-      <c r="F40" s="31" t="s">
-        <v>18</v>
-      </c>
-      <c r="G40" s="32"/>
-    </row>
-    <row r="41" ht="19.5" customHeight="1" spans="1:7">
-      <c r="A41" s="15">
-        <v>28</v>
-      </c>
-      <c r="B41" s="17"/>
-      <c r="C41" s="17"/>
-      <c r="D41" s="17"/>
-      <c r="E41" s="15"/>
-      <c r="F41" s="31" t="s">
-        <v>18</v>
-      </c>
-      <c r="G41" s="32"/>
-    </row>
-    <row r="42" ht="19.5" customHeight="1" spans="1:7">
-      <c r="A42" s="15">
-        <v>29</v>
-      </c>
-      <c r="B42" s="17"/>
-      <c r="C42" s="17"/>
-      <c r="D42" s="17"/>
-      <c r="E42" s="15"/>
-      <c r="F42" s="31" t="s">
-        <v>18</v>
-      </c>
-      <c r="G42" s="32"/>
-    </row>
-    <row r="43" ht="19.5" customHeight="1" spans="1:7">
-      <c r="A43" s="15">
-        <v>30</v>
-      </c>
-      <c r="B43" s="17"/>
-      <c r="C43" s="17"/>
-      <c r="D43" s="17"/>
-      <c r="E43" s="15"/>
-      <c r="F43" s="31" t="s">
-        <v>18</v>
-      </c>
-      <c r="G43" s="32"/>
-    </row>
-    <row r="44" ht="19.5" customHeight="1" spans="1:7">
-      <c r="A44" s="15">
-        <v>31</v>
-      </c>
-      <c r="B44" s="17"/>
-      <c r="C44" s="17"/>
-      <c r="D44" s="17"/>
-      <c r="E44" s="15"/>
-      <c r="F44" s="31" t="s">
-        <v>18</v>
-      </c>
-      <c r="G44" s="32"/>
-    </row>
-    <row r="45" ht="19.5" customHeight="1" spans="1:3">
-      <c r="A45" s="18"/>
-      <c r="B45" s="18"/>
-      <c r="C45" s="18"/>
-    </row>
-    <row r="46" ht="19.5" customHeight="1" spans="3:5">
-      <c r="C46" s="19" t="s">
-        <v>19</v>
-      </c>
-      <c r="D46" s="20"/>
-      <c r="E46" s="33">
-        <f>SUM(C14:C45)</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="47" ht="19.5" customHeight="1"/>
-    <row r="48" ht="57.75" customHeight="1"/>
-    <row r="49" ht="12.75" customHeight="1" spans="3:5">
-      <c r="C49" s="21" t="s">
-        <v>20</v>
-      </c>
-      <c r="D49" s="22"/>
-      <c r="E49" s="34"/>
-    </row>
-    <row r="50" ht="12.75" customHeight="1" spans="3:5">
-      <c r="C50" s="23"/>
-      <c r="D50" s="22"/>
-      <c r="E50" s="34"/>
-    </row>
-    <row r="51" ht="12.75" customHeight="1"/>
-    <row r="52" ht="12.75" customHeight="1"/>
+      <c r="D52" s="23"/>
+      <c r="E52" s="23"/>
+      <c r="F52" s="33"/>
+    </row>
     <row r="53" ht="12.75" customHeight="1" spans="3:6">
-      <c r="C53" s="24" t="s">
-        <v>21</v>
-      </c>
+      <c r="C53" s="24"/>
       <c r="D53" s="25"/>
       <c r="E53" s="25"/>
-      <c r="F53" s="35"/>
-    </row>
-    <row r="54" ht="12.75" customHeight="1" spans="3:6">
-      <c r="C54" s="26"/>
-      <c r="D54" s="27"/>
-      <c r="E54" s="27"/>
-      <c r="F54" s="36"/>
-    </row>
-    <row r="55" ht="12.75" customHeight="1"/>
+      <c r="F53" s="34"/>
+    </row>
+    <row r="54" ht="12.75" customHeight="1"/>
+    <row r="55" ht="12.75" customHeight="1" spans="3:6">
+      <c r="C55" s="22" t="s">
+        <v>21</v>
+      </c>
+      <c r="D55" s="23"/>
+      <c r="E55" s="23"/>
+      <c r="F55" s="33"/>
+    </row>
     <row r="56" ht="12.75" customHeight="1" spans="3:6">
-      <c r="C56" s="24" t="s">
-        <v>22</v>
-      </c>
-      <c r="D56" s="25"/>
-      <c r="E56" s="25"/>
+      <c r="C56" s="24"/>
+      <c r="D56" s="26"/>
+      <c r="E56" s="26"/>
       <c r="F56" s="35"/>
     </row>
-    <row r="57" ht="12.75" customHeight="1" spans="3:6">
-      <c r="C57" s="26"/>
-      <c r="D57" s="28"/>
-      <c r="E57" s="28"/>
-      <c r="F57" s="37"/>
-    </row>
+    <row r="57" ht="12.75" customHeight="1"/>
     <row r="58" ht="12.75" customHeight="1"/>
     <row r="59" ht="12.75" customHeight="1"/>
     <row r="60" ht="12.75" customHeight="1"/>
@@ -3149,7 +3116,7 @@
     <row r="1009" ht="15.75" customHeight="1"/>
     <row r="1010" ht="15.75" customHeight="1"/>
   </sheetData>
-  <mergeCells count="27">
+  <mergeCells count="25">
     <mergeCell ref="A1:G1"/>
     <mergeCell ref="A2:G2"/>
     <mergeCell ref="A3:B3"/>
@@ -3168,15 +3135,13 @@
     <mergeCell ref="C9:G9"/>
     <mergeCell ref="A10:B10"/>
     <mergeCell ref="C10:G10"/>
-    <mergeCell ref="A11:B11"/>
-    <mergeCell ref="C11:G11"/>
-    <mergeCell ref="C46:D46"/>
+    <mergeCell ref="C45:D45"/>
+    <mergeCell ref="C48:E48"/>
     <mergeCell ref="C49:E49"/>
-    <mergeCell ref="C50:E50"/>
+    <mergeCell ref="C52:F52"/>
     <mergeCell ref="C53:F53"/>
-    <mergeCell ref="C54:F54"/>
+    <mergeCell ref="C55:F55"/>
     <mergeCell ref="C56:F56"/>
-    <mergeCell ref="C57:F57"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0" footer="0"/>
   <pageSetup paperSize="9" scale="56" orientation="portrait"/>

</xml_diff>